<commit_message>
Adding all the files I need for the presentation.
</commit_message>
<xml_diff>
--- a/Miscellaneous/results.xlsx
+++ b/Miscellaneous/results.xlsx
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +57,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,13 +87,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +920,7 @@
         <v>3.8100000000000023</v>
       </c>
     </row>
-    <row r="33" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H33">
         <v>197.63499999999999</v>
       </c>
@@ -922,7 +937,7 @@
         <v>8.0649999999999977</v>
       </c>
     </row>
-    <row r="34" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H34">
         <v>205.7</v>
       </c>
@@ -939,7 +954,7 @@
         <v>8.0649999999999977</v>
       </c>
     </row>
-    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H35">
         <v>213.76499999999999</v>
       </c>
@@ -956,7 +971,7 @@
         <v>8.0649999999999977</v>
       </c>
     </row>
-    <row r="36" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H36">
         <v>221.83</v>
       </c>
@@ -973,7 +988,7 @@
         <v>8.0649999999999977</v>
       </c>
     </row>
-    <row r="37" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H37">
         <v>229.89500000000001</v>
       </c>
@@ -990,7 +1005,7 @@
         <v>8.0650000000000261</v>
       </c>
     </row>
-    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H38">
         <v>233.70500000000001</v>
       </c>
@@ -1007,7 +1022,7 @@
         <v>8.0649999999999977</v>
       </c>
     </row>
-    <row r="39" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H39">
         <v>241.77</v>
       </c>
@@ -1024,7 +1039,7 @@
         <v>3.8100000000000023</v>
       </c>
     </row>
-    <row r="40" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H40">
         <v>249.83500000000001</v>
       </c>
@@ -1040,8 +1055,12 @@
         <f t="shared" si="1"/>
         <v>8.0649999999999977</v>
       </c>
-    </row>
-    <row r="41" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <f>8.3*6</f>
+        <v>49.800000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H41">
         <v>257.89999999999998</v>
       </c>
@@ -1057,8 +1076,16 @@
         <f t="shared" si="1"/>
         <v>8.0649999999999977</v>
       </c>
-    </row>
-    <row r="42" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <f>SUM(K40:K45)</f>
+        <v>48.390000000000015</v>
+      </c>
+      <c r="O41">
+        <f>N41/5</f>
+        <v>9.6780000000000026</v>
+      </c>
+    </row>
+    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H42">
         <v>265.96499999999997</v>
       </c>
@@ -1070,7 +1097,7 @@
         <f>H41</f>
         <v>257.89999999999998</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="1">
         <f t="shared" si="1"/>
         <v>8.0649999999999693</v>
       </c>
@@ -1079,7 +1106,7 @@
         <v>16.129999999999967</v>
       </c>
     </row>
-    <row r="43" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H43">
         <v>274.02999999999997</v>
       </c>
@@ -1091,12 +1118,12 @@
         <f>H42</f>
         <v>265.96499999999997</v>
       </c>
-      <c r="K43">
-        <f t="shared" si="1"/>
-        <v>8.0649999999999977</v>
-      </c>
-    </row>
-    <row r="44" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="K43" s="1">
+        <f t="shared" si="1"/>
+        <v>8.0649999999999977</v>
+      </c>
+    </row>
+    <row r="44" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H44">
         <v>282.09500000000003</v>
       </c>
@@ -1113,7 +1140,7 @@
         <v>8.0649999999999977</v>
       </c>
     </row>
-    <row r="45" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H45">
         <v>285.90499999999997</v>
       </c>
@@ -1130,7 +1157,7 @@
         <v>8.0650000000000546</v>
       </c>
     </row>
-    <row r="46" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H46">
         <v>293.97000000000003</v>
       </c>
@@ -1147,7 +1174,7 @@
         <v>3.8099999999999454</v>
       </c>
     </row>
-    <row r="47" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H47">
         <v>302.03500000000003</v>
       </c>
@@ -1164,7 +1191,7 @@
         <v>8.0650000000000546</v>
       </c>
     </row>
-    <row r="48" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H48">
         <v>310.10000000000002</v>
       </c>

</xml_diff>

<commit_message>
Updating results spreadsheet with remaining p4 and p5 results.
</commit_message>
<xml_diff>
--- a/Miscellaneous/results.xlsx
+++ b/Miscellaneous/results.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="meshing stuff" sheetId="1" r:id="rId1"/>
+    <sheet name="p4 results" sheetId="2" r:id="rId2"/>
+    <sheet name="p5 results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>step pos</t>
   </si>
@@ -43,6 +43,51 @@
   </si>
   <si>
     <t>new delta</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>keff diff</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>outers</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>poly</t>
+  </si>
+  <si>
+    <t>subplane</t>
+  </si>
+  <si>
+    <t>cpm</t>
+  </si>
+  <si>
+    <t>rms</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>CMFD iters</t>
   </si>
 </sst>
 </file>
@@ -91,9 +136,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -398,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -488,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J62" si="0">H7</f>
+        <f t="shared" ref="J7" si="0">H7</f>
         <v>0</v>
       </c>
       <c r="K7">
@@ -521,7 +568,7 @@
         <v>3.8659999999999997</v>
       </c>
       <c r="J9">
-        <f>H8</f>
+        <f t="shared" ref="J9:J40" si="3">H8</f>
         <v>11.951000000000001</v>
       </c>
       <c r="K9">
@@ -538,7 +585,7 @@
         <v>8.2109999999999985</v>
       </c>
       <c r="J10">
-        <f>H9</f>
+        <f t="shared" si="3"/>
         <v>15.817</v>
       </c>
       <c r="K10">
@@ -555,7 +602,7 @@
         <v>8.2109999999999985</v>
       </c>
       <c r="J11">
-        <f>H10</f>
+        <f t="shared" si="3"/>
         <v>24.027999999999999</v>
       </c>
       <c r="K11">
@@ -572,7 +619,7 @@
         <v>8.2110000000000056</v>
       </c>
       <c r="J12">
-        <f>H11</f>
+        <f t="shared" si="3"/>
         <v>32.238999999999997</v>
       </c>
       <c r="K12">
@@ -589,7 +636,7 @@
         <v>8.2119999999999962</v>
       </c>
       <c r="J13">
-        <f>H12</f>
+        <f t="shared" si="3"/>
         <v>40.450000000000003</v>
       </c>
       <c r="K13">
@@ -606,7 +653,7 @@
         <v>8.2109999999999985</v>
       </c>
       <c r="J14">
-        <f>H13</f>
+        <f t="shared" si="3"/>
         <v>48.661999999999999</v>
       </c>
       <c r="K14">
@@ -623,7 +670,7 @@
         <v>8.2110000000000056</v>
       </c>
       <c r="J15">
-        <f>H14</f>
+        <f t="shared" si="3"/>
         <v>56.872999999999998</v>
       </c>
       <c r="K15">
@@ -640,7 +687,7 @@
         <v>8.2109999999999985</v>
       </c>
       <c r="J16">
-        <f>H15</f>
+        <f t="shared" si="3"/>
         <v>65.084000000000003</v>
       </c>
       <c r="K16">
@@ -657,7 +704,7 @@
         <v>3.8100000000000023</v>
       </c>
       <c r="J17">
-        <f>H16</f>
+        <f t="shared" si="3"/>
         <v>73.295000000000002</v>
       </c>
       <c r="K17">
@@ -674,7 +721,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J18">
-        <f>H17</f>
+        <f t="shared" si="3"/>
         <v>77.105000000000004</v>
       </c>
       <c r="K18">
@@ -691,7 +738,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J19">
-        <f>H18</f>
+        <f t="shared" si="3"/>
         <v>85.17</v>
       </c>
       <c r="K19">
@@ -708,7 +755,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J20">
-        <f>H19</f>
+        <f t="shared" si="3"/>
         <v>93.234999999999999</v>
       </c>
       <c r="K20">
@@ -725,7 +772,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J21">
-        <f>H20</f>
+        <f t="shared" si="3"/>
         <v>101.3</v>
       </c>
       <c r="K21">
@@ -742,7 +789,7 @@
         <v>8.0650000000000119</v>
       </c>
       <c r="J22">
-        <f>H21</f>
+        <f t="shared" si="3"/>
         <v>109.36499999999999</v>
       </c>
       <c r="K22">
@@ -759,7 +806,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J23">
-        <f>H22</f>
+        <f t="shared" si="3"/>
         <v>117.43</v>
       </c>
       <c r="K23">
@@ -776,7 +823,7 @@
         <v>3.8100000000000023</v>
       </c>
       <c r="J24">
-        <f>H23</f>
+        <f t="shared" si="3"/>
         <v>125.495</v>
       </c>
       <c r="K24">
@@ -793,7 +840,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J25">
-        <f>H24</f>
+        <f t="shared" si="3"/>
         <v>129.30500000000001</v>
       </c>
       <c r="K25">
@@ -810,7 +857,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J26">
-        <f>H25</f>
+        <f t="shared" si="3"/>
         <v>137.37</v>
       </c>
       <c r="K26">
@@ -827,7 +874,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J27">
-        <f>H26</f>
+        <f t="shared" si="3"/>
         <v>145.435</v>
       </c>
       <c r="K27">
@@ -844,7 +891,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J28">
-        <f>H27</f>
+        <f t="shared" si="3"/>
         <v>153.5</v>
       </c>
       <c r="K28">
@@ -861,7 +908,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J29">
-        <f>H28</f>
+        <f t="shared" si="3"/>
         <v>161.565</v>
       </c>
       <c r="K29">
@@ -878,7 +925,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J30">
-        <f>H29</f>
+        <f t="shared" si="3"/>
         <v>169.63</v>
       </c>
       <c r="K30">
@@ -895,7 +942,7 @@
         <v>3.8100000000000023</v>
       </c>
       <c r="J31">
-        <f>H30</f>
+        <f t="shared" si="3"/>
         <v>177.69499999999999</v>
       </c>
       <c r="K31">
@@ -912,7 +959,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J32">
-        <f>H31</f>
+        <f t="shared" si="3"/>
         <v>181.505</v>
       </c>
       <c r="K32">
@@ -929,7 +976,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J33">
-        <f>H32</f>
+        <f t="shared" si="3"/>
         <v>189.57</v>
       </c>
       <c r="K33">
@@ -946,7 +993,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J34">
-        <f>H33</f>
+        <f t="shared" si="3"/>
         <v>197.63499999999999</v>
       </c>
       <c r="K34">
@@ -963,7 +1010,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J35">
-        <f>H34</f>
+        <f t="shared" si="3"/>
         <v>205.7</v>
       </c>
       <c r="K35">
@@ -980,7 +1027,7 @@
         <v>8.0650000000000261</v>
       </c>
       <c r="J36">
-        <f>H35</f>
+        <f t="shared" si="3"/>
         <v>213.76499999999999</v>
       </c>
       <c r="K36">
@@ -997,7 +1044,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J37">
-        <f>H36</f>
+        <f t="shared" si="3"/>
         <v>221.83</v>
       </c>
       <c r="K37">
@@ -1014,7 +1061,7 @@
         <v>3.8100000000000023</v>
       </c>
       <c r="J38">
-        <f>H37</f>
+        <f t="shared" si="3"/>
         <v>229.89500000000001</v>
       </c>
       <c r="K38">
@@ -1031,7 +1078,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J39">
-        <f>H38</f>
+        <f t="shared" si="3"/>
         <v>233.70500000000001</v>
       </c>
       <c r="K39">
@@ -1048,7 +1095,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J40">
-        <f>H39</f>
+        <f t="shared" si="3"/>
         <v>241.77</v>
       </c>
       <c r="K40">
@@ -1069,7 +1116,7 @@
         <v>8.0649999999999693</v>
       </c>
       <c r="J41">
-        <f>H40</f>
+        <f t="shared" ref="J41:J58" si="4">H40</f>
         <v>249.83500000000001</v>
       </c>
       <c r="K41">
@@ -1094,7 +1141,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J42">
-        <f>H41</f>
+        <f t="shared" si="4"/>
         <v>257.89999999999998</v>
       </c>
       <c r="K42" s="1">
@@ -1115,7 +1162,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J43">
-        <f>H42</f>
+        <f t="shared" si="4"/>
         <v>265.96499999999997</v>
       </c>
       <c r="K43" s="1">
@@ -1132,7 +1179,7 @@
         <v>8.0650000000000546</v>
       </c>
       <c r="J44">
-        <f>H43</f>
+        <f t="shared" si="4"/>
         <v>274.02999999999997</v>
       </c>
       <c r="K44">
@@ -1149,7 +1196,7 @@
         <v>3.8099999999999454</v>
       </c>
       <c r="J45">
-        <f>H44</f>
+        <f t="shared" si="4"/>
         <v>282.09500000000003</v>
       </c>
       <c r="K45">
@@ -1166,7 +1213,7 @@
         <v>8.0650000000000546</v>
       </c>
       <c r="J46">
-        <f>H45</f>
+        <f t="shared" si="4"/>
         <v>285.90499999999997</v>
       </c>
       <c r="K46">
@@ -1183,7 +1230,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J47">
-        <f>H46</f>
+        <f t="shared" si="4"/>
         <v>293.97000000000003</v>
       </c>
       <c r="K47">
@@ -1200,7 +1247,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J48">
-        <f>H47</f>
+        <f t="shared" si="4"/>
         <v>302.03500000000003</v>
       </c>
       <c r="K48">
@@ -1217,7 +1264,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J49">
-        <f>H48</f>
+        <f t="shared" si="4"/>
         <v>310.10000000000002</v>
       </c>
       <c r="K49">
@@ -1234,7 +1281,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J50">
-        <f>H49</f>
+        <f t="shared" si="4"/>
         <v>318.16500000000002</v>
       </c>
       <c r="K50">
@@ -1251,7 +1298,7 @@
         <v>8.0649999999999977</v>
       </c>
       <c r="J51">
-        <f>H50</f>
+        <f t="shared" si="4"/>
         <v>326.23</v>
       </c>
       <c r="K51">
@@ -1268,7 +1315,7 @@
         <v>3.8100000000000023</v>
       </c>
       <c r="J52">
-        <f>H51</f>
+        <f t="shared" si="4"/>
         <v>334.29500000000002</v>
       </c>
       <c r="K52">
@@ -1285,7 +1332,7 @@
         <v>7.9211999999999989</v>
       </c>
       <c r="J53">
-        <f>H52</f>
+        <f t="shared" si="4"/>
         <v>338.10500000000002</v>
       </c>
       <c r="K53">
@@ -1302,7 +1349,7 @@
         <v>7.9211999999999989</v>
       </c>
       <c r="J54">
-        <f>H53</f>
+        <f t="shared" si="4"/>
         <v>346.02620000000002</v>
       </c>
       <c r="K54">
@@ -1319,7 +1366,7 @@
         <v>7.9211999999999989</v>
       </c>
       <c r="J55">
-        <f>H54</f>
+        <f t="shared" si="4"/>
         <v>353.94740000000002</v>
       </c>
       <c r="K55">
@@ -1336,7 +1383,7 @@
         <v>7.9211999999999989</v>
       </c>
       <c r="J56">
-        <f>H55</f>
+        <f t="shared" si="4"/>
         <v>361.86860000000001</v>
       </c>
       <c r="K56">
@@ -1353,7 +1400,7 @@
         <v>7.9211999999999989</v>
       </c>
       <c r="J57">
-        <f>H56</f>
+        <f t="shared" si="4"/>
         <v>369.78980000000001</v>
       </c>
       <c r="K57">
@@ -1370,7 +1417,7 @@
         <v>16</v>
       </c>
       <c r="J58">
-        <f>H57</f>
+        <f t="shared" si="4"/>
         <v>377.71100000000001</v>
       </c>
       <c r="K58">
@@ -1431,7 +1478,7 @@
     </row>
     <row r="62" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H62">
-        <f t="shared" ref="H62" si="3">H61+I62</f>
+        <f t="shared" ref="H62" si="5">H61+I62</f>
         <v>413.93700000000001</v>
       </c>
       <c r="I62">
@@ -1473,24 +1520,369 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>517</v>
+      </c>
+      <c r="G3">
+        <f>8*60+50</f>
+        <v>530</v>
+      </c>
+      <c r="H3">
+        <f>G3/G$3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-30.280929</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.8360999999999999E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.218083</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>512</v>
+      </c>
+      <c r="G4">
+        <f>10*60+4</f>
+        <v>604</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H7" si="0">G4/G$3</f>
+        <v>1.1396226415094339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-7.9185299999999996</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.0293E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.5757999999999997E-2</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>506</v>
+      </c>
+      <c r="G5">
+        <f>10*60+8</f>
+        <v>608</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.1471698113207547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-7.3639460000000003</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.1278E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.1148000000000003E-2</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>525</v>
+      </c>
+      <c r="G6">
+        <f>9*60+58</f>
+        <v>598</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.1283018867924528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-1.5902670000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.4019999999999997E-3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.9576000000000002E-2</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>526</v>
+      </c>
+      <c r="G7">
+        <f>10*60+11</f>
+        <v>611</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.1528301886792454</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B4:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>445</v>
+      </c>
+      <c r="G3">
+        <v>383.3</v>
+      </c>
+      <c r="H3">
+        <f>G3/G$3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-22</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="E4">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>546</v>
+      </c>
+      <c r="G4">
+        <v>439.8</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H7" si="0">G4/G$3</f>
+        <v>1.1474041220975737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.18E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.1178</v>
+      </c>
+      <c r="E5">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>495</v>
+      </c>
+      <c r="G5">
+        <v>407.4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.0628750326115313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.1206</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>517</v>
+      </c>
+      <c r="G6">
+        <v>424.3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.1069658231150534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-1.0293129999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.09E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.1217</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>525</v>
+      </c>
+      <c r="G7">
+        <f>(60*27+24)/3600*912</f>
+        <v>416.48</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.0865640490477433</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating results spreadsheet with p5 results and p4 plane 32 results
</commit_message>
<xml_diff>
--- a/Miscellaneous/results.xlsx
+++ b/Miscellaneous/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meshing stuff" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="28">
   <si>
     <t>step pos</t>
   </si>
@@ -100,13 +100,19 @@
   <si>
     <t>core-hours</t>
   </si>
+  <si>
+    <t>Plane 32 only</t>
+  </si>
+  <si>
+    <t>Plane 32 Only</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.##\%;[Red]\(0.##\%\)"/>
+    <numFmt numFmtId="164" formatCode="0.##\%;[Red]\(0.##\%\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -154,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1572,15 +1578,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1605,16 +1611,43 @@
       <c r="I1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1645,8 +1678,14 @@
         <f>G3/G$3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1677,8 +1716,38 @@
         <f t="shared" ref="I4:I7" si="0">G4/G$3</f>
         <v>1.0938086303939962</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4">
+        <v>12</v>
+      </c>
+      <c r="R4">
+        <v>364</v>
+      </c>
+      <c r="S4">
+        <f>8*60+53</f>
+        <v>533</v>
+      </c>
+      <c r="T4">
+        <f>S4/3600*58</f>
+        <v>8.5872222222222216</v>
+      </c>
+      <c r="U4">
+        <f>S4/S$4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1709,8 +1778,38 @@
         <f t="shared" si="0"/>
         <v>1.125703564727955</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="2">
+        <v>-30.279947</v>
+      </c>
+      <c r="O5" s="3">
+        <v>10.225394</v>
+      </c>
+      <c r="P5" s="3">
+        <v>21.808522</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <v>352</v>
+      </c>
+      <c r="S5">
+        <f>9*60+43</f>
+        <v>583</v>
+      </c>
+      <c r="T5">
+        <f>S5/3600*57</f>
+        <v>9.230833333333333</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U8" si="2">S5/S$4</f>
+        <v>1.0938086303939962</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1741,8 +1840,38 @@
         <f t="shared" si="0"/>
         <v>1.0975609756097562</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="2">
+        <v>-7.9190300000000002</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1.9159550000000001</v>
+      </c>
+      <c r="P6" s="3">
+        <v>4.0437399999999997</v>
+      </c>
+      <c r="Q6">
+        <v>12</v>
+      </c>
+      <c r="R6">
+        <v>360</v>
+      </c>
+      <c r="S6">
+        <f>60*10</f>
+        <v>600</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6:T8" si="3">S6/3600*57</f>
+        <v>9.5</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="2"/>
+        <v>1.125703564727955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1773,8 +1902,70 @@
         <f t="shared" si="0"/>
         <v>1.1200750469043153</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="2">
+        <v>-7.3641290000000001</v>
+      </c>
+      <c r="O7" s="3">
+        <v>3.0639630000000002</v>
+      </c>
+      <c r="P7" s="3">
+        <v>7.1148569999999998</v>
+      </c>
+      <c r="Q7">
+        <v>12</v>
+      </c>
+      <c r="R7">
+        <v>409</v>
+      </c>
+      <c r="S7">
+        <f>9*60+45</f>
+        <v>585</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>9.2625000000000011</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>1.0975609756097562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="2">
+        <v>-1.5908469999999999</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.74074600000000002</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1.90605</v>
+      </c>
+      <c r="Q8">
+        <v>12</v>
+      </c>
+      <c r="R8">
+        <v>364</v>
+      </c>
+      <c r="S8">
+        <f>9*60+57</f>
+        <v>597</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>9.4525000000000006</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>1.1200750469043153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>24</v>
       </c>
@@ -1792,7 +1983,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>24</v>
       </c>
@@ -1806,7 +1997,7 @@
         <v>6.4640099999999994E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>24</v>
       </c>
@@ -1820,7 +2011,7 @@
         <v>8.4208090000000004E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>24</v>
       </c>
@@ -1834,7 +2025,7 @@
         <v>3.7241299999999999E-8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -1848,7 +2039,7 @@
         <v>9.5857079999999995E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -1862,7 +2053,7 @@
         <v>6.37067E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>24</v>
       </c>
@@ -1954,155 +2145,580 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="E3">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <f>G3/3600*928</f>
-        <v>0</v>
-      </c>
-      <c r="I3" t="e">
-        <f>G3/G$3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
-        <v>-22</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
       <c r="E4">
         <v>13</v>
       </c>
+      <c r="F4">
+        <v>481</v>
+      </c>
+      <c r="G4">
+        <f>23*60+23</f>
+        <v>1403</v>
+      </c>
       <c r="H4">
-        <f>G4/3600*912</f>
-        <v>0</v>
-      </c>
-      <c r="I4" t="e">
-        <f t="shared" ref="I4:I7" si="0">G4/G$3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <f>G4/3600*928</f>
+        <v>361.66222222222223</v>
+      </c>
+      <c r="I4">
+        <f>G4/G$4</f>
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4">
+        <v>13</v>
+      </c>
+      <c r="Q4">
+        <v>481</v>
+      </c>
+      <c r="R4">
+        <f>23*60+23</f>
+        <v>1403</v>
+      </c>
+      <c r="S4">
+        <f>R4/3600*928</f>
+        <v>361.66222222222223</v>
+      </c>
+      <c r="T4">
+        <f>R4/R$4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>-5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+        <v>-22.264810000000001</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.900919</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30.553343000000002</v>
+      </c>
       <c r="E5">
         <v>13</v>
       </c>
+      <c r="F5">
+        <v>523</v>
+      </c>
+      <c r="G5">
+        <f>27*60+1</f>
+        <v>1621</v>
+      </c>
       <c r="H5">
-        <f t="shared" ref="H5:H7" si="1">G5/3600*912</f>
-        <v>0</v>
-      </c>
-      <c r="I5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <f>G5/3600*912</f>
+        <v>410.65333333333331</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I8" si="0">G5/G$4</f>
+        <v>1.1553813257305774</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="2">
+        <v>-22.264810000000001</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2.8189519999999999</v>
+      </c>
+      <c r="O5" s="3">
+        <v>30.553343000000002</v>
+      </c>
+      <c r="P5">
+        <v>13</v>
+      </c>
+      <c r="Q5">
+        <v>523</v>
+      </c>
+      <c r="R5">
+        <f>27*60+1</f>
+        <v>1621</v>
+      </c>
+      <c r="S5">
+        <f>R5/3600*912</f>
+        <v>410.65333333333331</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T8" si="1">R5/R$4</f>
+        <v>1.1553813257305774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
-        <v>-5</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+        <v>-5.1143239999999999</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.152733</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.854304</v>
+      </c>
       <c r="E6">
         <v>13</v>
       </c>
+      <c r="F6">
+        <v>463</v>
+      </c>
+      <c r="G6">
+        <f>24*60+35</f>
+        <v>1475</v>
+      </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6" t="e">
+        <f t="shared" ref="H6:H8" si="2">G6/3600*912</f>
+        <v>373.66666666666663</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0513186029935853</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="2">
+        <v>-5.1143239999999999</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1.1736180000000001</v>
+      </c>
+      <c r="O6" s="3">
+        <v>11.678881000000001</v>
+      </c>
+      <c r="P6">
+        <v>13</v>
+      </c>
+      <c r="Q6">
+        <v>463</v>
+      </c>
+      <c r="R6">
+        <f>24*60+35</f>
+        <v>1475</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S8" si="3">R6/3600*912</f>
+        <v>373.66666666666663</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>1.0513186029935853</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
-        <v>-1.0293129999999999</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>-5.4258959999999998</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.0894400000000002</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10.198798999999999</v>
+      </c>
       <c r="E7">
         <v>13</v>
       </c>
+      <c r="F7">
+        <v>499</v>
+      </c>
+      <c r="G7">
+        <f>26*60+15</f>
+        <v>1575</v>
+      </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I7" t="e">
+        <f t="shared" si="2"/>
+        <v>399</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.1225944404846757</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="2">
+        <v>-5.4258959999999998</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1.26616</v>
+      </c>
+      <c r="O7" s="3">
+        <v>11.956996999999999</v>
+      </c>
+      <c r="P7">
+        <v>13</v>
+      </c>
+      <c r="Q7">
+        <v>499</v>
+      </c>
+      <c r="R7">
+        <f>26*60+15</f>
+        <v>1575</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>399</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>1.1225944404846757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-1.032327</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.49898999999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.73943</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>529</v>
+      </c>
+      <c r="G8">
+        <f>28*60</f>
+        <v>1680</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>425.6</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.1974340698503207</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="2">
+        <v>-1.032327</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1.0774539999999999</v>
+      </c>
+      <c r="O8" s="3">
+        <v>12.069520000000001</v>
+      </c>
+      <c r="P8">
+        <v>13</v>
+      </c>
+      <c r="Q8">
+        <v>529</v>
+      </c>
+      <c r="R8">
+        <f>28*60</f>
+        <v>1680</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>425.6</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>1.1974340698503207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>0.98769079999999998</v>
+      </c>
+      <c r="F12" s="4">
+        <v>6.1640040000000001E-8</v>
+      </c>
+      <c r="I12">
+        <f>SUM(D12:D23)</f>
+        <v>523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>57</v>
+      </c>
+      <c r="E13">
+        <v>0.99256230000000001</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5.343676E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>61</v>
+      </c>
+      <c r="E14">
+        <v>0.99800650000000002</v>
+      </c>
+      <c r="F14" s="4">
+        <v>7.9180239999999995E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>59</v>
+      </c>
+      <c r="E15">
+        <v>0.99775510000000001</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4.0140489999999998E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>71</v>
+      </c>
+      <c r="E16">
+        <v>0.99811740000000004</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3.9053360000000001E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>38</v>
+      </c>
+      <c r="E17">
+        <v>0.99817730000000005</v>
+      </c>
+      <c r="F17" s="4">
+        <v>8.1016599999999995E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>34</v>
+      </c>
+      <c r="E18">
+        <v>0.99824080000000004</v>
+      </c>
+      <c r="F18" s="4">
+        <v>9.9382290000000003E-8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>0.99826060000000005</v>
+      </c>
+      <c r="F19" s="4">
+        <v>8.9499990000000004E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>0.99826910000000002</v>
+      </c>
+      <c r="F20" s="4">
+        <v>8.9642899999999999E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>0.9982721</v>
+      </c>
+      <c r="F21" s="4">
+        <v>8.0065990000000001E-8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>0.99827399999999999</v>
+      </c>
+      <c r="F22" s="4">
+        <v>8.7254529999999999E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>0.99827509999999997</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5.828055E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>0.99827569999999999</v>
+      </c>
+      <c r="F24" s="4">
+        <v>9.4141739999999993E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some tables for 3D core results
</commit_message>
<xml_diff>
--- a/Miscellaneous/results.xlsx
+++ b/Miscellaneous/results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarog\dissertation\Miscellaneous\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-225" yWindow="-165" windowWidth="27795" windowHeight="14310" activeTab="6"/>
+    <workbookView xWindow="-225" yWindow="-165" windowWidth="27795" windowHeight="14310" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="meshing stuff" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="3D Subray" sheetId="7" r:id="rId7"/>
     <sheet name="3D Subray Runtime" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -533,7 +538,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.##\%;[Red]\(0.##\%\)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -727,22 +732,25 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -763,13 +771,10 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -835,7 +840,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,9 +873,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -903,6 +925,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3560,48 +3599,48 @@
       <c r="J14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="46" t="s">
+      <c r="K14" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="48" t="s">
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="46" t="s">
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T14" s="46"/>
-      <c r="U14" s="46"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="48" t="s">
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="48"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="46" t="s">
+      <c r="X14" s="46"/>
+      <c r="Y14" s="46"/>
+      <c r="Z14" s="46"/>
+      <c r="AA14" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB14" s="46"/>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="46"/>
-      <c r="AE14" s="48" t="s">
+      <c r="AB14" s="48"/>
+      <c r="AC14" s="48"/>
+      <c r="AD14" s="48"/>
+      <c r="AE14" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF14" s="48"/>
-      <c r="AG14" s="48"/>
-      <c r="AH14" s="48"/>
-      <c r="AI14" s="46" t="s">
+      <c r="AF14" s="46"/>
+      <c r="AG14" s="46"/>
+      <c r="AH14" s="46"/>
+      <c r="AI14" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ14" s="46"/>
-      <c r="AK14" s="46"/>
-      <c r="AL14" s="46"/>
+      <c r="AJ14" s="48"/>
+      <c r="AK14" s="48"/>
+      <c r="AL14" s="48"/>
     </row>
     <row r="15" spans="4:38" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
@@ -3614,58 +3653,58 @@
         <v>41</v>
       </c>
       <c r="L15" s="47"/>
-      <c r="M15" s="49" t="s">
+      <c r="M15" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="49"/>
+      <c r="N15" s="51"/>
       <c r="O15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P15" s="50"/>
-      <c r="Q15" s="48" t="s">
+      <c r="Q15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="48"/>
+      <c r="R15" s="46"/>
       <c r="S15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T15" s="47"/>
-      <c r="U15" s="46" t="s">
+      <c r="U15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V15" s="46"/>
+      <c r="V15" s="48"/>
       <c r="W15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X15" s="50"/>
-      <c r="Y15" s="48" t="s">
+      <c r="Y15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z15" s="48"/>
+      <c r="Z15" s="46"/>
       <c r="AA15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB15" s="47"/>
-      <c r="AC15" s="46" t="s">
+      <c r="AC15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD15" s="46"/>
+      <c r="AD15" s="48"/>
       <c r="AE15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF15" s="50"/>
-      <c r="AG15" s="48" t="s">
+      <c r="AG15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH15" s="48"/>
+      <c r="AH15" s="46"/>
       <c r="AI15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ15" s="47"/>
-      <c r="AK15" s="46" t="s">
+      <c r="AK15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL15" s="46"/>
+      <c r="AL15" s="48"/>
     </row>
     <row r="16" spans="4:38" x14ac:dyDescent="0.25">
       <c r="J16" s="8" t="s">
@@ -3757,13 +3796,13 @@
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="51"/>
+      <c r="D17" s="49"/>
       <c r="I17">
         <v>0</v>
       </c>
@@ -3818,7 +3857,7 @@
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B18" s="51"/>
+      <c r="B18" s="49"/>
       <c r="C18" t="s">
         <v>39</v>
       </c>
@@ -4835,48 +4874,48 @@
       <c r="J32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="46" t="s">
+      <c r="K32" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="48" t="s">
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
-      <c r="R32" s="48"/>
-      <c r="S32" s="46" t="s">
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
-      <c r="V32" s="46"/>
-      <c r="W32" s="48" t="s">
+      <c r="T32" s="48"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="48"/>
+      <c r="W32" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X32" s="48"/>
-      <c r="Y32" s="48"/>
-      <c r="Z32" s="48"/>
-      <c r="AA32" s="46" t="s">
+      <c r="X32" s="46"/>
+      <c r="Y32" s="46"/>
+      <c r="Z32" s="46"/>
+      <c r="AA32" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB32" s="46"/>
-      <c r="AC32" s="46"/>
-      <c r="AD32" s="46"/>
-      <c r="AE32" s="48" t="s">
+      <c r="AB32" s="48"/>
+      <c r="AC32" s="48"/>
+      <c r="AD32" s="48"/>
+      <c r="AE32" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF32" s="48"/>
-      <c r="AG32" s="48"/>
-      <c r="AH32" s="48"/>
-      <c r="AI32" s="46" t="s">
+      <c r="AF32" s="46"/>
+      <c r="AG32" s="46"/>
+      <c r="AH32" s="46"/>
+      <c r="AI32" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ32" s="46"/>
-      <c r="AK32" s="46"/>
-      <c r="AL32" s="46"/>
+      <c r="AJ32" s="48"/>
+      <c r="AK32" s="48"/>
+      <c r="AL32" s="48"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
@@ -4889,58 +4928,58 @@
         <v>41</v>
       </c>
       <c r="L33" s="47"/>
-      <c r="M33" s="49" t="s">
+      <c r="M33" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N33" s="49"/>
+      <c r="N33" s="51"/>
       <c r="O33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P33" s="50"/>
-      <c r="Q33" s="48" t="s">
+      <c r="Q33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R33" s="48"/>
+      <c r="R33" s="46"/>
       <c r="S33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T33" s="47"/>
-      <c r="U33" s="46" t="s">
+      <c r="U33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V33" s="46"/>
+      <c r="V33" s="48"/>
       <c r="W33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X33" s="50"/>
-      <c r="Y33" s="48" t="s">
+      <c r="Y33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z33" s="48"/>
+      <c r="Z33" s="46"/>
       <c r="AA33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB33" s="47"/>
-      <c r="AC33" s="46" t="s">
+      <c r="AC33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD33" s="46"/>
+      <c r="AD33" s="48"/>
       <c r="AE33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF33" s="50"/>
-      <c r="AG33" s="48" t="s">
+      <c r="AG33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH33" s="48"/>
+      <c r="AH33" s="46"/>
       <c r="AI33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ33" s="47"/>
-      <c r="AK33" s="46" t="s">
+      <c r="AK33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL33" s="46"/>
+      <c r="AL33" s="48"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J34" s="8" t="s">
@@ -5032,13 +5071,13 @@
       </c>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="51"/>
+      <c r="D35" s="49"/>
       <c r="I35">
         <v>0</v>
       </c>
@@ -5138,7 +5177,7 @@
       </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B36" s="51"/>
+      <c r="B36" s="49"/>
       <c r="C36" t="s">
         <v>39</v>
       </c>
@@ -6445,48 +6484,48 @@
       <c r="J51" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K51" s="46" t="s">
+      <c r="K51" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L51" s="46"/>
-      <c r="M51" s="46"/>
-      <c r="N51" s="46"/>
-      <c r="O51" s="48" t="s">
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P51" s="48"/>
-      <c r="Q51" s="48"/>
-      <c r="R51" s="48"/>
-      <c r="S51" s="46" t="s">
+      <c r="P51" s="46"/>
+      <c r="Q51" s="46"/>
+      <c r="R51" s="46"/>
+      <c r="S51" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T51" s="46"/>
-      <c r="U51" s="46"/>
-      <c r="V51" s="46"/>
-      <c r="W51" s="48" t="s">
+      <c r="T51" s="48"/>
+      <c r="U51" s="48"/>
+      <c r="V51" s="48"/>
+      <c r="W51" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X51" s="48"/>
-      <c r="Y51" s="48"/>
-      <c r="Z51" s="48"/>
-      <c r="AA51" s="46" t="s">
+      <c r="X51" s="46"/>
+      <c r="Y51" s="46"/>
+      <c r="Z51" s="46"/>
+      <c r="AA51" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB51" s="46"/>
-      <c r="AC51" s="46"/>
-      <c r="AD51" s="46"/>
-      <c r="AE51" s="48" t="s">
+      <c r="AB51" s="48"/>
+      <c r="AC51" s="48"/>
+      <c r="AD51" s="48"/>
+      <c r="AE51" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF51" s="48"/>
-      <c r="AG51" s="48"/>
-      <c r="AH51" s="48"/>
-      <c r="AI51" s="46" t="s">
+      <c r="AF51" s="46"/>
+      <c r="AG51" s="46"/>
+      <c r="AH51" s="46"/>
+      <c r="AI51" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ51" s="46"/>
-      <c r="AK51" s="46"/>
-      <c r="AL51" s="46"/>
+      <c r="AJ51" s="48"/>
+      <c r="AK51" s="48"/>
+      <c r="AL51" s="48"/>
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
@@ -6499,58 +6538,58 @@
         <v>41</v>
       </c>
       <c r="L52" s="47"/>
-      <c r="M52" s="49" t="s">
+      <c r="M52" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N52" s="49"/>
+      <c r="N52" s="51"/>
       <c r="O52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P52" s="50"/>
-      <c r="Q52" s="48" t="s">
+      <c r="Q52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R52" s="48"/>
+      <c r="R52" s="46"/>
       <c r="S52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T52" s="47"/>
-      <c r="U52" s="46" t="s">
+      <c r="U52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V52" s="46"/>
+      <c r="V52" s="48"/>
       <c r="W52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X52" s="50"/>
-      <c r="Y52" s="48" t="s">
+      <c r="Y52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z52" s="48"/>
+      <c r="Z52" s="46"/>
       <c r="AA52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB52" s="47"/>
-      <c r="AC52" s="46" t="s">
+      <c r="AC52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD52" s="46"/>
+      <c r="AD52" s="48"/>
       <c r="AE52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF52" s="50"/>
-      <c r="AG52" s="48" t="s">
+      <c r="AG52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH52" s="48"/>
+      <c r="AH52" s="46"/>
       <c r="AI52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ52" s="47"/>
-      <c r="AK52" s="46" t="s">
+      <c r="AK52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL52" s="46"/>
+      <c r="AL52" s="48"/>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J53" s="8" t="s">
@@ -6642,13 +6681,13 @@
       </c>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B54" s="51" t="s">
+      <c r="B54" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="C54" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="51"/>
+      <c r="D54" s="49"/>
       <c r="I54">
         <v>0</v>
       </c>
@@ -6748,7 +6787,7 @@
       </c>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B55" s="51"/>
+      <c r="B55" s="49"/>
       <c r="C55" t="s">
         <v>39</v>
       </c>
@@ -8055,48 +8094,48 @@
       <c r="J70" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K70" s="46" t="s">
+      <c r="K70" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L70" s="46"/>
-      <c r="M70" s="46"/>
-      <c r="N70" s="46"/>
-      <c r="O70" s="48" t="s">
+      <c r="L70" s="48"/>
+      <c r="M70" s="48"/>
+      <c r="N70" s="48"/>
+      <c r="O70" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P70" s="48"/>
-      <c r="Q70" s="48"/>
-      <c r="R70" s="48"/>
-      <c r="S70" s="46" t="s">
+      <c r="P70" s="46"/>
+      <c r="Q70" s="46"/>
+      <c r="R70" s="46"/>
+      <c r="S70" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T70" s="46"/>
-      <c r="U70" s="46"/>
-      <c r="V70" s="46"/>
-      <c r="W70" s="48" t="s">
+      <c r="T70" s="48"/>
+      <c r="U70" s="48"/>
+      <c r="V70" s="48"/>
+      <c r="W70" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X70" s="48"/>
-      <c r="Y70" s="48"/>
-      <c r="Z70" s="48"/>
-      <c r="AA70" s="46" t="s">
+      <c r="X70" s="46"/>
+      <c r="Y70" s="46"/>
+      <c r="Z70" s="46"/>
+      <c r="AA70" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB70" s="46"/>
-      <c r="AC70" s="46"/>
-      <c r="AD70" s="46"/>
-      <c r="AE70" s="48" t="s">
+      <c r="AB70" s="48"/>
+      <c r="AC70" s="48"/>
+      <c r="AD70" s="48"/>
+      <c r="AE70" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF70" s="48"/>
-      <c r="AG70" s="48"/>
-      <c r="AH70" s="48"/>
-      <c r="AI70" s="46" t="s">
+      <c r="AF70" s="46"/>
+      <c r="AG70" s="46"/>
+      <c r="AH70" s="46"/>
+      <c r="AI70" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ70" s="46"/>
-      <c r="AK70" s="46"/>
-      <c r="AL70" s="46"/>
+      <c r="AJ70" s="48"/>
+      <c r="AK70" s="48"/>
+      <c r="AL70" s="48"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
@@ -8109,58 +8148,58 @@
         <v>41</v>
       </c>
       <c r="L71" s="47"/>
-      <c r="M71" s="49" t="s">
+      <c r="M71" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N71" s="49"/>
+      <c r="N71" s="51"/>
       <c r="O71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P71" s="50"/>
-      <c r="Q71" s="48" t="s">
+      <c r="Q71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R71" s="48"/>
+      <c r="R71" s="46"/>
       <c r="S71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T71" s="47"/>
-      <c r="U71" s="46" t="s">
+      <c r="U71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V71" s="46"/>
+      <c r="V71" s="48"/>
       <c r="W71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X71" s="50"/>
-      <c r="Y71" s="48" t="s">
+      <c r="Y71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z71" s="48"/>
+      <c r="Z71" s="46"/>
       <c r="AA71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB71" s="47"/>
-      <c r="AC71" s="46" t="s">
+      <c r="AC71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD71" s="46"/>
+      <c r="AD71" s="48"/>
       <c r="AE71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF71" s="50"/>
-      <c r="AG71" s="48" t="s">
+      <c r="AG71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH71" s="48"/>
+      <c r="AH71" s="46"/>
       <c r="AI71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ71" s="47"/>
-      <c r="AK71" s="46" t="s">
+      <c r="AK71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL71" s="46"/>
+      <c r="AL71" s="48"/>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J72" s="8" t="s">
@@ -8252,13 +8291,13 @@
       </c>
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B73" s="51" t="s">
+      <c r="B73" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="51" t="s">
+      <c r="C73" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="51"/>
+      <c r="D73" s="49"/>
       <c r="I73">
         <v>0</v>
       </c>
@@ -8358,7 +8397,7 @@
       </c>
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B74" s="51"/>
+      <c r="B74" s="49"/>
       <c r="C74" t="s">
         <v>39</v>
       </c>
@@ -9660,6 +9699,82 @@
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AE32:AH32"/>
+    <mergeCell ref="AI32:AL32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AC33:AD33"/>
+    <mergeCell ref="AG33:AH33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:Z32"/>
+    <mergeCell ref="AA32:AD32"/>
+    <mergeCell ref="AE51:AH51"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AE33:AF33"/>
+    <mergeCell ref="Y52:Z52"/>
+    <mergeCell ref="AA52:AB52"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="S51:V51"/>
+    <mergeCell ref="W51:Z51"/>
+    <mergeCell ref="AA51:AD51"/>
+    <mergeCell ref="AE14:AH14"/>
+    <mergeCell ref="AI14:AL14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="W14:Z14"/>
+    <mergeCell ref="AA14:AD14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="O70:R70"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AC52:AD52"/>
+    <mergeCell ref="AE52:AF52"/>
+    <mergeCell ref="AG52:AH52"/>
+    <mergeCell ref="AI52:AJ52"/>
+    <mergeCell ref="AK52:AL52"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="W52:X52"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="S70:V70"/>
+    <mergeCell ref="W70:Z70"/>
+    <mergeCell ref="AA70:AD70"/>
+    <mergeCell ref="AE70:AH70"/>
+    <mergeCell ref="AI70:AL70"/>
     <mergeCell ref="AG71:AH71"/>
     <mergeCell ref="AI71:AJ71"/>
     <mergeCell ref="AK71:AL71"/>
@@ -9676,82 +9791,6 @@
     <mergeCell ref="O71:P71"/>
     <mergeCell ref="Q71:R71"/>
     <mergeCell ref="S71:T71"/>
-    <mergeCell ref="S70:V70"/>
-    <mergeCell ref="W70:Z70"/>
-    <mergeCell ref="AA70:AD70"/>
-    <mergeCell ref="AE70:AH70"/>
-    <mergeCell ref="AI70:AL70"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="O70:R70"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AC52:AD52"/>
-    <mergeCell ref="AE52:AF52"/>
-    <mergeCell ref="AG52:AH52"/>
-    <mergeCell ref="AI52:AJ52"/>
-    <mergeCell ref="AK52:AL52"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="W52:X52"/>
-    <mergeCell ref="AE14:AH14"/>
-    <mergeCell ref="AI14:AL14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W14:Z14"/>
-    <mergeCell ref="AA14:AD14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="Y52:Z52"/>
-    <mergeCell ref="AA52:AB52"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="O51:R51"/>
-    <mergeCell ref="S51:V51"/>
-    <mergeCell ref="W51:Z51"/>
-    <mergeCell ref="AA51:AD51"/>
-    <mergeCell ref="AE51:AH51"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AE33:AF33"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AE32:AH32"/>
-    <mergeCell ref="AI32:AL32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AC33:AD33"/>
-    <mergeCell ref="AG33:AH33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="O32:R32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:Z32"/>
-    <mergeCell ref="AA32:AD32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9802,137 +9841,137 @@
         <v>67</v>
       </c>
       <c r="M1" s="59"/>
-      <c r="N1" s="60" t="s">
+      <c r="N1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="48" t="s">
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="60" t="s">
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="48" t="s">
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="60" t="s">
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="48" t="s">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="60" t="s">
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="60"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L2" s="58" t="s">
+      <c r="L2" s="60" t="s">
         <v>65</v>
       </c>
       <c r="M2" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="53" t="s">
+      <c r="O2" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="54" t="s">
+      <c r="P2" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="55" t="s">
+      <c r="Q2" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="56" t="s">
+      <c r="R2" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="52" t="s">
+      <c r="T2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="53" t="s">
+      <c r="U2" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="54" t="s">
+      <c r="V2" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="W2" s="55" t="s">
+      <c r="W2" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="57" t="s">
+      <c r="Y2" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="52" t="s">
+      <c r="Z2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="54" t="s">
+      <c r="AB2" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="55" t="s">
+      <c r="AC2" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="AD2" s="56" t="s">
+      <c r="AD2" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="AE2" s="57" t="s">
+      <c r="AE2" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AF2" s="52" t="s">
+      <c r="AF2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="AH2" s="54" t="s">
+      <c r="AH2" s="55" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L3" s="58"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="59"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="54"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="55"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="55"/>
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="57"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="54"/>
+      <c r="AH3" s="55"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="K4">
@@ -11298,41 +11337,41 @@
         <v>67</v>
       </c>
       <c r="M21" s="59"/>
-      <c r="N21" s="60" t="s">
+      <c r="N21" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="48" t="s">
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="60" t="s">
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="U21" s="60"/>
-      <c r="V21" s="60"/>
-      <c r="W21" s="48" t="s">
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="60" t="s">
+      <c r="X21" s="46"/>
+      <c r="Y21" s="46"/>
+      <c r="Z21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="AA21" s="60"/>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="48" t="s">
+      <c r="AA21" s="52"/>
+      <c r="AB21" s="52"/>
+      <c r="AC21" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AD21" s="48"/>
-      <c r="AE21" s="48"/>
-      <c r="AF21" s="60" t="s">
+      <c r="AD21" s="46"/>
+      <c r="AE21" s="46"/>
+      <c r="AF21" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="AG21" s="60"/>
-      <c r="AH21" s="60"/>
+      <c r="AG21" s="52"/>
+      <c r="AH21" s="52"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -11356,73 +11395,73 @@
         <f t="shared" si="1"/>
         <v>649.29999999999995</v>
       </c>
-      <c r="L22" s="58" t="s">
+      <c r="L22" s="60" t="s">
         <v>65</v>
       </c>
       <c r="M22" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="52" t="s">
+      <c r="N22" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="O22" s="53" t="s">
+      <c r="O22" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="P22" s="54" t="s">
+      <c r="P22" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="Q22" s="55" t="s">
+      <c r="Q22" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="R22" s="56" t="s">
+      <c r="R22" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="S22" s="57" t="s">
+      <c r="S22" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="T22" s="52" t="s">
+      <c r="T22" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="U22" s="53" t="s">
+      <c r="U22" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="V22" s="54" t="s">
+      <c r="V22" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="W22" s="55" t="s">
+      <c r="W22" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="X22" s="56" t="s">
+      <c r="X22" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="Y22" s="57" t="s">
+      <c r="Y22" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="Z22" s="52" t="s">
+      <c r="Z22" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AA22" s="53" t="s">
+      <c r="AA22" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="AB22" s="54" t="s">
+      <c r="AB22" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="AC22" s="55" t="s">
+      <c r="AC22" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="AD22" s="56" t="s">
+      <c r="AD22" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="AE22" s="57" t="s">
+      <c r="AE22" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AF22" s="52" t="s">
+      <c r="AF22" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AG22" s="53" t="s">
+      <c r="AG22" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="AH22" s="54" t="s">
+      <c r="AH22" s="55" t="s">
         <v>68</v>
       </c>
     </row>
@@ -11448,29 +11487,29 @@
         <f t="shared" si="1"/>
         <v>665.8</v>
       </c>
-      <c r="L23" s="58"/>
+      <c r="L23" s="60"/>
       <c r="M23" s="59"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="53"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="55"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="57"/>
-      <c r="Z23" s="52"/>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="54"/>
-      <c r="AC23" s="55"/>
-      <c r="AD23" s="56"/>
-      <c r="AE23" s="57"/>
-      <c r="AF23" s="52"/>
-      <c r="AG23" s="53"/>
-      <c r="AH23" s="54"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="53"/>
+      <c r="AA23" s="54"/>
+      <c r="AB23" s="55"/>
+      <c r="AC23" s="56"/>
+      <c r="AD23" s="57"/>
+      <c r="AE23" s="58"/>
+      <c r="AF23" s="53"/>
+      <c r="AG23" s="54"/>
+      <c r="AH23" s="55"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -12843,41 +12882,41 @@
         <v>67</v>
       </c>
       <c r="M42" s="59"/>
-      <c r="N42" s="60" t="s">
+      <c r="N42" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="O42" s="60"/>
-      <c r="P42" s="60"/>
-      <c r="Q42" s="48" t="s">
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+      <c r="Q42" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="R42" s="48"/>
-      <c r="S42" s="48"/>
-      <c r="T42" s="60" t="s">
+      <c r="R42" s="46"/>
+      <c r="S42" s="46"/>
+      <c r="T42" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="U42" s="60"/>
-      <c r="V42" s="60"/>
-      <c r="W42" s="48" t="s">
+      <c r="U42" s="52"/>
+      <c r="V42" s="52"/>
+      <c r="W42" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X42" s="48"/>
-      <c r="Y42" s="48"/>
-      <c r="Z42" s="60" t="s">
+      <c r="X42" s="46"/>
+      <c r="Y42" s="46"/>
+      <c r="Z42" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="AA42" s="60"/>
-      <c r="AB42" s="60"/>
-      <c r="AC42" s="48" t="s">
+      <c r="AA42" s="52"/>
+      <c r="AB42" s="52"/>
+      <c r="AC42" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AD42" s="48"/>
-      <c r="AE42" s="48"/>
-      <c r="AF42" s="60" t="s">
+      <c r="AD42" s="46"/>
+      <c r="AE42" s="46"/>
+      <c r="AF42" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="AG42" s="60"/>
-      <c r="AH42" s="60"/>
+      <c r="AG42" s="52"/>
+      <c r="AH42" s="52"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -12901,73 +12940,73 @@
         <f t="shared" si="1"/>
         <v>1005.61</v>
       </c>
-      <c r="L43" s="58" t="s">
+      <c r="L43" s="60" t="s">
         <v>65</v>
       </c>
       <c r="M43" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N43" s="52" t="s">
+      <c r="N43" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="53" t="s">
+      <c r="O43" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="P43" s="54" t="s">
+      <c r="P43" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="Q43" s="55" t="s">
+      <c r="Q43" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="R43" s="56" t="s">
+      <c r="R43" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="S43" s="57" t="s">
+      <c r="S43" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="T43" s="52" t="s">
+      <c r="T43" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="U43" s="53" t="s">
+      <c r="U43" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="V43" s="54" t="s">
+      <c r="V43" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="W43" s="55" t="s">
+      <c r="W43" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="X43" s="56" t="s">
+      <c r="X43" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="Y43" s="57" t="s">
+      <c r="Y43" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="Z43" s="52" t="s">
+      <c r="Z43" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AA43" s="53" t="s">
+      <c r="AA43" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="AB43" s="54" t="s">
+      <c r="AB43" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="AC43" s="55" t="s">
+      <c r="AC43" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="AD43" s="56" t="s">
+      <c r="AD43" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="AE43" s="57" t="s">
+      <c r="AE43" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AF43" s="52" t="s">
+      <c r="AF43" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AG43" s="53" t="s">
+      <c r="AG43" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="AH43" s="54" t="s">
+      <c r="AH43" s="55" t="s">
         <v>68</v>
       </c>
     </row>
@@ -12993,29 +13032,29 @@
         <f t="shared" si="1"/>
         <v>1050.77</v>
       </c>
-      <c r="L44" s="58"/>
+      <c r="L44" s="60"/>
       <c r="M44" s="59"/>
-      <c r="N44" s="52"/>
-      <c r="O44" s="53"/>
-      <c r="P44" s="54"/>
-      <c r="Q44" s="55"/>
-      <c r="R44" s="56"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="52"/>
-      <c r="U44" s="53"/>
-      <c r="V44" s="54"/>
-      <c r="W44" s="55"/>
-      <c r="X44" s="56"/>
-      <c r="Y44" s="57"/>
-      <c r="Z44" s="52"/>
-      <c r="AA44" s="53"/>
-      <c r="AB44" s="54"/>
-      <c r="AC44" s="55"/>
-      <c r="AD44" s="56"/>
-      <c r="AE44" s="57"/>
-      <c r="AF44" s="52"/>
-      <c r="AG44" s="53"/>
-      <c r="AH44" s="54"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="54"/>
+      <c r="P44" s="55"/>
+      <c r="Q44" s="56"/>
+      <c r="R44" s="57"/>
+      <c r="S44" s="58"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="54"/>
+      <c r="V44" s="55"/>
+      <c r="W44" s="56"/>
+      <c r="X44" s="57"/>
+      <c r="Y44" s="58"/>
+      <c r="Z44" s="53"/>
+      <c r="AA44" s="54"/>
+      <c r="AB44" s="55"/>
+      <c r="AC44" s="56"/>
+      <c r="AD44" s="57"/>
+      <c r="AE44" s="58"/>
+      <c r="AF44" s="53"/>
+      <c r="AG44" s="54"/>
+      <c r="AH44" s="55"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -15025,44 +15064,45 @@
     <sortCondition ref="C5:C48"/>
   </sortState>
   <mergeCells count="93">
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:Y21"/>
-    <mergeCell ref="Z21:AB21"/>
-    <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="AF43:AF44"/>
+    <mergeCell ref="AG43:AG44"/>
+    <mergeCell ref="AH43:AH44"/>
+    <mergeCell ref="AA43:AA44"/>
+    <mergeCell ref="AB43:AB44"/>
+    <mergeCell ref="AC43:AC44"/>
+    <mergeCell ref="AD43:AD44"/>
+    <mergeCell ref="AE43:AE44"/>
+    <mergeCell ref="V43:V44"/>
+    <mergeCell ref="W43:W44"/>
+    <mergeCell ref="X43:X44"/>
+    <mergeCell ref="Y43:Y44"/>
+    <mergeCell ref="Z43:Z44"/>
+    <mergeCell ref="Q43:Q44"/>
+    <mergeCell ref="R43:R44"/>
+    <mergeCell ref="S43:S44"/>
+    <mergeCell ref="T43:T44"/>
+    <mergeCell ref="U43:U44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="AF22:AF23"/>
+    <mergeCell ref="AG22:AG23"/>
+    <mergeCell ref="AH22:AH23"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="T42:V42"/>
+    <mergeCell ref="W42:Y42"/>
+    <mergeCell ref="Z42:AB42"/>
+    <mergeCell ref="AC42:AE42"/>
+    <mergeCell ref="AF42:AH42"/>
+    <mergeCell ref="AA22:AA23"/>
+    <mergeCell ref="AB22:AB23"/>
+    <mergeCell ref="AC22:AC23"/>
+    <mergeCell ref="AD22:AD23"/>
+    <mergeCell ref="AE22:AE23"/>
     <mergeCell ref="AF21:AH21"/>
     <mergeCell ref="L22:L23"/>
     <mergeCell ref="M22:M23"/>
@@ -15079,45 +15119,44 @@
     <mergeCell ref="X22:X23"/>
     <mergeCell ref="Y22:Y23"/>
     <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="AF22:AF23"/>
-    <mergeCell ref="AG22:AG23"/>
-    <mergeCell ref="AH22:AH23"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:P42"/>
-    <mergeCell ref="Q42:S42"/>
-    <mergeCell ref="T42:V42"/>
-    <mergeCell ref="W42:Y42"/>
-    <mergeCell ref="Z42:AB42"/>
-    <mergeCell ref="AC42:AE42"/>
-    <mergeCell ref="AF42:AH42"/>
-    <mergeCell ref="AA22:AA23"/>
-    <mergeCell ref="AB22:AB23"/>
-    <mergeCell ref="AC22:AC23"/>
-    <mergeCell ref="AD22:AD23"/>
-    <mergeCell ref="AE22:AE23"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="P43:P44"/>
-    <mergeCell ref="Q43:Q44"/>
-    <mergeCell ref="R43:R44"/>
-    <mergeCell ref="S43:S44"/>
-    <mergeCell ref="T43:T44"/>
-    <mergeCell ref="U43:U44"/>
-    <mergeCell ref="V43:V44"/>
-    <mergeCell ref="W43:W44"/>
-    <mergeCell ref="X43:X44"/>
-    <mergeCell ref="Y43:Y44"/>
-    <mergeCell ref="Z43:Z44"/>
-    <mergeCell ref="AF43:AF44"/>
-    <mergeCell ref="AG43:AG44"/>
-    <mergeCell ref="AH43:AH44"/>
-    <mergeCell ref="AA43:AA44"/>
-    <mergeCell ref="AB43:AB44"/>
-    <mergeCell ref="AC43:AC44"/>
-    <mergeCell ref="AD43:AD44"/>
-    <mergeCell ref="AE43:AE44"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="Z21:AB21"/>
+    <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15506,8 +15545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AL119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AJ117" sqref="AJ117:AL118"/>
+    <sheetView topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D94" sqref="A88:D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15522,48 +15561,48 @@
       <c r="J4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="48" t="s">
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="46" t="s">
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-      <c r="W4" s="48" t="s">
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="46" t="s">
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="46"/>
-      <c r="AE4" s="48" t="s">
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF4" s="48"/>
-      <c r="AG4" s="48"/>
-      <c r="AH4" s="48"/>
-      <c r="AI4" s="46" t="s">
+      <c r="AF4" s="46"/>
+      <c r="AG4" s="46"/>
+      <c r="AH4" s="46"/>
+      <c r="AI4" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ4" s="46"/>
-      <c r="AK4" s="46"/>
-      <c r="AL4" s="46"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="48"/>
+      <c r="AL4" s="48"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
@@ -15576,58 +15615,58 @@
         <v>41</v>
       </c>
       <c r="L5" s="47"/>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="49"/>
+      <c r="N5" s="51"/>
       <c r="O5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P5" s="50"/>
-      <c r="Q5" s="48" t="s">
+      <c r="Q5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="48"/>
+      <c r="R5" s="46"/>
       <c r="S5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T5" s="47"/>
-      <c r="U5" s="46" t="s">
+      <c r="U5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V5" s="46"/>
+      <c r="V5" s="48"/>
       <c r="W5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X5" s="50"/>
-      <c r="Y5" s="48" t="s">
+      <c r="Y5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="48"/>
+      <c r="Z5" s="46"/>
       <c r="AA5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB5" s="47"/>
-      <c r="AC5" s="46" t="s">
+      <c r="AC5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD5" s="46"/>
+      <c r="AD5" s="48"/>
       <c r="AE5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF5" s="50"/>
-      <c r="AG5" s="48" t="s">
+      <c r="AG5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH5" s="48"/>
+      <c r="AH5" s="46"/>
       <c r="AI5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ5" s="47"/>
-      <c r="AK5" s="46" t="s">
+      <c r="AK5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL5" s="46"/>
+      <c r="AL5" s="48"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J6" s="8" t="s">
@@ -15719,13 +15758,13 @@
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="49"/>
       <c r="I7">
         <v>0</v>
       </c>
@@ -15825,7 +15864,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
+      <c r="B8" s="49"/>
       <c r="C8" t="s">
         <v>39</v>
       </c>
@@ -18972,48 +19011,48 @@
       <c r="J43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K43" s="46" t="s">
+      <c r="K43" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L43" s="46"/>
-      <c r="M43" s="46"/>
-      <c r="N43" s="46"/>
-      <c r="O43" s="48" t="s">
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="S43" s="46" t="s">
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T43" s="46"/>
-      <c r="U43" s="46"/>
-      <c r="V43" s="46"/>
-      <c r="W43" s="48" t="s">
+      <c r="T43" s="48"/>
+      <c r="U43" s="48"/>
+      <c r="V43" s="48"/>
+      <c r="W43" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X43" s="48"/>
-      <c r="Y43" s="48"/>
-      <c r="Z43" s="48"/>
-      <c r="AA43" s="46" t="s">
+      <c r="X43" s="46"/>
+      <c r="Y43" s="46"/>
+      <c r="Z43" s="46"/>
+      <c r="AA43" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB43" s="46"/>
-      <c r="AC43" s="46"/>
-      <c r="AD43" s="46"/>
-      <c r="AE43" s="48" t="s">
+      <c r="AB43" s="48"/>
+      <c r="AC43" s="48"/>
+      <c r="AD43" s="48"/>
+      <c r="AE43" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF43" s="48"/>
-      <c r="AG43" s="48"/>
-      <c r="AH43" s="48"/>
-      <c r="AI43" s="46" t="s">
+      <c r="AF43" s="46"/>
+      <c r="AG43" s="46"/>
+      <c r="AH43" s="46"/>
+      <c r="AI43" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ43" s="46"/>
-      <c r="AK43" s="46"/>
-      <c r="AL43" s="46"/>
+      <c r="AJ43" s="48"/>
+      <c r="AK43" s="48"/>
+      <c r="AL43" s="48"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
@@ -19026,58 +19065,58 @@
         <v>41</v>
       </c>
       <c r="L44" s="47"/>
-      <c r="M44" s="49" t="s">
+      <c r="M44" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N44" s="49"/>
+      <c r="N44" s="51"/>
       <c r="O44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P44" s="50"/>
-      <c r="Q44" s="48" t="s">
+      <c r="Q44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R44" s="48"/>
+      <c r="R44" s="46"/>
       <c r="S44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T44" s="47"/>
-      <c r="U44" s="46" t="s">
+      <c r="U44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V44" s="46"/>
+      <c r="V44" s="48"/>
       <c r="W44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X44" s="50"/>
-      <c r="Y44" s="48" t="s">
+      <c r="Y44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z44" s="48"/>
+      <c r="Z44" s="46"/>
       <c r="AA44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB44" s="47"/>
-      <c r="AC44" s="46" t="s">
+      <c r="AC44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD44" s="46"/>
+      <c r="AD44" s="48"/>
       <c r="AE44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF44" s="50"/>
-      <c r="AG44" s="48" t="s">
+      <c r="AG44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH44" s="48"/>
+      <c r="AH44" s="46"/>
       <c r="AI44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ44" s="47"/>
-      <c r="AK44" s="46" t="s">
+      <c r="AK44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL44" s="46"/>
+      <c r="AL44" s="48"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J45" s="8" t="s">
@@ -19169,13 +19208,13 @@
       </c>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B46" s="51" t="s">
+      <c r="B46" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="51" t="s">
+      <c r="C46" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="51"/>
+      <c r="D46" s="49"/>
       <c r="I46">
         <v>0</v>
       </c>
@@ -19275,7 +19314,7 @@
       </c>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B47" s="51"/>
+      <c r="B47" s="49"/>
       <c r="C47" t="s">
         <v>39</v>
       </c>
@@ -22330,48 +22369,48 @@
       <c r="J83" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K83" s="46" t="s">
+      <c r="K83" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="L83" s="46"/>
-      <c r="M83" s="46"/>
-      <c r="N83" s="46"/>
-      <c r="O83" s="48" t="s">
+      <c r="L83" s="48"/>
+      <c r="M83" s="48"/>
+      <c r="N83" s="48"/>
+      <c r="O83" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P83" s="48"/>
-      <c r="Q83" s="48"/>
-      <c r="R83" s="48"/>
-      <c r="S83" s="46" t="s">
+      <c r="P83" s="46"/>
+      <c r="Q83" s="46"/>
+      <c r="R83" s="46"/>
+      <c r="S83" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T83" s="46"/>
-      <c r="U83" s="46"/>
-      <c r="V83" s="46"/>
-      <c r="W83" s="48" t="s">
+      <c r="T83" s="48"/>
+      <c r="U83" s="48"/>
+      <c r="V83" s="48"/>
+      <c r="W83" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="X83" s="48"/>
-      <c r="Y83" s="48"/>
-      <c r="Z83" s="48"/>
-      <c r="AA83" s="46" t="s">
+      <c r="X83" s="46"/>
+      <c r="Y83" s="46"/>
+      <c r="Z83" s="46"/>
+      <c r="AA83" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="AB83" s="46"/>
-      <c r="AC83" s="46"/>
-      <c r="AD83" s="46"/>
-      <c r="AE83" s="48" t="s">
+      <c r="AB83" s="48"/>
+      <c r="AC83" s="48"/>
+      <c r="AD83" s="48"/>
+      <c r="AE83" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF83" s="48"/>
-      <c r="AG83" s="48"/>
-      <c r="AH83" s="48"/>
-      <c r="AI83" s="46" t="s">
+      <c r="AF83" s="46"/>
+      <c r="AG83" s="46"/>
+      <c r="AH83" s="46"/>
+      <c r="AI83" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AJ83" s="46"/>
-      <c r="AK83" s="46"/>
-      <c r="AL83" s="46"/>
+      <c r="AJ83" s="48"/>
+      <c r="AK83" s="48"/>
+      <c r="AL83" s="48"/>
     </row>
     <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H84" t="s">
@@ -22384,58 +22423,58 @@
         <v>41</v>
       </c>
       <c r="L84" s="47"/>
-      <c r="M84" s="49" t="s">
+      <c r="M84" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="N84" s="49"/>
+      <c r="N84" s="51"/>
       <c r="O84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P84" s="50"/>
-      <c r="Q84" s="48" t="s">
+      <c r="Q84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="R84" s="48"/>
+      <c r="R84" s="46"/>
       <c r="S84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T84" s="47"/>
-      <c r="U84" s="46" t="s">
+      <c r="U84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="V84" s="46"/>
+      <c r="V84" s="48"/>
       <c r="W84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X84" s="50"/>
-      <c r="Y84" s="48" t="s">
+      <c r="Y84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="Z84" s="48"/>
+      <c r="Z84" s="46"/>
       <c r="AA84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB84" s="47"/>
-      <c r="AC84" s="46" t="s">
+      <c r="AC84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AD84" s="46"/>
+      <c r="AD84" s="48"/>
       <c r="AE84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF84" s="50"/>
-      <c r="AG84" s="48" t="s">
+      <c r="AG84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AH84" s="48"/>
+      <c r="AH84" s="46"/>
       <c r="AI84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ84" s="47"/>
-      <c r="AK84" s="46" t="s">
+      <c r="AK84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL84" s="46"/>
+      <c r="AL84" s="48"/>
     </row>
     <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J85" s="8" t="s">
@@ -22527,13 +22566,13 @@
       </c>
     </row>
     <row r="86" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B86" s="51" t="s">
+      <c r="B86" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C86" s="51" t="s">
+      <c r="C86" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D86" s="51"/>
+      <c r="D86" s="49"/>
       <c r="I86">
         <v>0</v>
       </c>
@@ -22633,7 +22672,7 @@
       </c>
     </row>
     <row r="87" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B87" s="51"/>
+      <c r="B87" s="49"/>
       <c r="C87" t="s">
         <v>39</v>
       </c>
@@ -25687,6 +25726,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="AI4:AL4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="O43:R43"/>
+    <mergeCell ref="S43:V43"/>
+    <mergeCell ref="W43:Z43"/>
+    <mergeCell ref="AA43:AD43"/>
+    <mergeCell ref="AE43:AH43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="W44:X44"/>
+    <mergeCell ref="Y44:Z44"/>
+    <mergeCell ref="AA44:AB44"/>
+    <mergeCell ref="AC44:AD44"/>
+    <mergeCell ref="AE44:AF44"/>
+    <mergeCell ref="AG44:AH44"/>
+    <mergeCell ref="AI44:AJ44"/>
+    <mergeCell ref="AK44:AL44"/>
+    <mergeCell ref="AA84:AB84"/>
+    <mergeCell ref="AC84:AD84"/>
+    <mergeCell ref="AE84:AF84"/>
+    <mergeCell ref="AG84:AH84"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="O83:R83"/>
+    <mergeCell ref="S83:V83"/>
     <mergeCell ref="AI84:AJ84"/>
     <mergeCell ref="AK84:AL84"/>
     <mergeCell ref="B86:B87"/>
@@ -25703,59 +25795,6 @@
     <mergeCell ref="U84:V84"/>
     <mergeCell ref="W84:X84"/>
     <mergeCell ref="Y84:Z84"/>
-    <mergeCell ref="AA84:AB84"/>
-    <mergeCell ref="AC84:AD84"/>
-    <mergeCell ref="AE84:AF84"/>
-    <mergeCell ref="AG84:AH84"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="O83:R83"/>
-    <mergeCell ref="S83:V83"/>
-    <mergeCell ref="AE43:AH43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="W44:X44"/>
-    <mergeCell ref="Y44:Z44"/>
-    <mergeCell ref="AA44:AB44"/>
-    <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="AE44:AF44"/>
-    <mergeCell ref="AG44:AH44"/>
-    <mergeCell ref="AI44:AJ44"/>
-    <mergeCell ref="AK44:AL44"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="O43:R43"/>
-    <mergeCell ref="S43:V43"/>
-    <mergeCell ref="W43:Z43"/>
-    <mergeCell ref="AA43:AD43"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="AI4:AL4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25766,8 +25805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH128"/>
   <sheetViews>
-    <sheetView topLeftCell="B67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF88" sqref="AF88"/>
+    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M113" sqref="M113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32412,7 +32451,7 @@
         <v>27.833333333333332</v>
       </c>
       <c r="M74" s="2">
-        <f t="shared" ref="M74:O74" si="24">AVERAGE(M63:M71,M53:M61,M43:M51)</f>
+        <f t="shared" ref="M74:N74" si="24">AVERAGE(M63:M71,M53:M61,M43:M51)</f>
         <v>3156.0400000000009</v>
       </c>
       <c r="N74" s="29">
@@ -35743,11 +35782,11 @@
         <v>27.222222222222221</v>
       </c>
       <c r="M112" s="2">
-        <f t="shared" ref="M112:O112" si="36">AVERAGE(M101:M109,M91:M99,M81:M89)</f>
+        <f>AVERAGE(M101:M109,M91:M99,M81:M89)</f>
         <v>3346.3111764705882</v>
       </c>
       <c r="N112" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="M112:O112" si="36">AVERAGE(N101:N109,N91:N99,N81:N89)</f>
         <v>27.944444444444443</v>
       </c>
       <c r="O112" s="27">

</xml_diff>

<commit_message>
Some discussion changes in results section
</commit_message>
<xml_diff>
--- a/Miscellaneous/results.xlsx
+++ b/Miscellaneous/results.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarog\dissertation\Miscellaneous\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-225" yWindow="-165" windowWidth="27795" windowHeight="14310" firstSheet="1" activeTab="7"/>
   </bookViews>
@@ -538,7 +533,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.##\%;[Red]\(0.##\%\)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -732,25 +727,22 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -771,10 +763,13 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -840,7 +835,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,26 +868,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -925,23 +903,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3348,7 +3309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AL85"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -3599,48 +3560,48 @@
       <c r="J14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="46" t="s">
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="48" t="s">
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="46" t="s">
+      <c r="T14" s="46"/>
+      <c r="U14" s="46"/>
+      <c r="V14" s="46"/>
+      <c r="W14" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="48" t="s">
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB14" s="48"/>
-      <c r="AC14" s="48"/>
-      <c r="AD14" s="48"/>
-      <c r="AE14" s="46" t="s">
+      <c r="AB14" s="46"/>
+      <c r="AC14" s="46"/>
+      <c r="AD14" s="46"/>
+      <c r="AE14" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF14" s="46"/>
-      <c r="AG14" s="46"/>
-      <c r="AH14" s="46"/>
-      <c r="AI14" s="48" t="s">
+      <c r="AF14" s="48"/>
+      <c r="AG14" s="48"/>
+      <c r="AH14" s="48"/>
+      <c r="AI14" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ14" s="48"/>
-      <c r="AK14" s="48"/>
-      <c r="AL14" s="48"/>
+      <c r="AJ14" s="46"/>
+      <c r="AK14" s="46"/>
+      <c r="AL14" s="46"/>
     </row>
     <row r="15" spans="4:38" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
@@ -3653,58 +3614,58 @@
         <v>41</v>
       </c>
       <c r="L15" s="47"/>
-      <c r="M15" s="51" t="s">
+      <c r="M15" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="51"/>
+      <c r="N15" s="49"/>
       <c r="O15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P15" s="50"/>
-      <c r="Q15" s="46" t="s">
+      <c r="Q15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="46"/>
+      <c r="R15" s="48"/>
       <c r="S15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T15" s="47"/>
-      <c r="U15" s="48" t="s">
+      <c r="U15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V15" s="48"/>
+      <c r="V15" s="46"/>
       <c r="W15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X15" s="50"/>
-      <c r="Y15" s="46" t="s">
+      <c r="Y15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z15" s="46"/>
+      <c r="Z15" s="48"/>
       <c r="AA15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB15" s="47"/>
-      <c r="AC15" s="48" t="s">
+      <c r="AC15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD15" s="48"/>
+      <c r="AD15" s="46"/>
       <c r="AE15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF15" s="50"/>
-      <c r="AG15" s="46" t="s">
+      <c r="AG15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH15" s="46"/>
+      <c r="AH15" s="48"/>
       <c r="AI15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ15" s="47"/>
-      <c r="AK15" s="48" t="s">
+      <c r="AK15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL15" s="48"/>
+      <c r="AL15" s="46"/>
     </row>
     <row r="16" spans="4:38" x14ac:dyDescent="0.25">
       <c r="J16" s="8" t="s">
@@ -3796,13 +3757,13 @@
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="51"/>
       <c r="I17">
         <v>0</v>
       </c>
@@ -3857,7 +3818,7 @@
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B18" s="49"/>
+      <c r="B18" s="51"/>
       <c r="C18" t="s">
         <v>39</v>
       </c>
@@ -4874,48 +4835,48 @@
       <c r="J32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="48" t="s">
+      <c r="K32" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="46" t="s">
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="48" t="s">
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T32" s="48"/>
-      <c r="U32" s="48"/>
-      <c r="V32" s="48"/>
-      <c r="W32" s="46" t="s">
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X32" s="46"/>
-      <c r="Y32" s="46"/>
-      <c r="Z32" s="46"/>
-      <c r="AA32" s="48" t="s">
+      <c r="X32" s="48"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="48"/>
+      <c r="AA32" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB32" s="48"/>
-      <c r="AC32" s="48"/>
-      <c r="AD32" s="48"/>
-      <c r="AE32" s="46" t="s">
+      <c r="AB32" s="46"/>
+      <c r="AC32" s="46"/>
+      <c r="AD32" s="46"/>
+      <c r="AE32" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF32" s="46"/>
-      <c r="AG32" s="46"/>
-      <c r="AH32" s="46"/>
-      <c r="AI32" s="48" t="s">
+      <c r="AF32" s="48"/>
+      <c r="AG32" s="48"/>
+      <c r="AH32" s="48"/>
+      <c r="AI32" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ32" s="48"/>
-      <c r="AK32" s="48"/>
-      <c r="AL32" s="48"/>
+      <c r="AJ32" s="46"/>
+      <c r="AK32" s="46"/>
+      <c r="AL32" s="46"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
@@ -4928,58 +4889,58 @@
         <v>41</v>
       </c>
       <c r="L33" s="47"/>
-      <c r="M33" s="51" t="s">
+      <c r="M33" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N33" s="51"/>
+      <c r="N33" s="49"/>
       <c r="O33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P33" s="50"/>
-      <c r="Q33" s="46" t="s">
+      <c r="Q33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R33" s="46"/>
+      <c r="R33" s="48"/>
       <c r="S33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T33" s="47"/>
-      <c r="U33" s="48" t="s">
+      <c r="U33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V33" s="48"/>
+      <c r="V33" s="46"/>
       <c r="W33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X33" s="50"/>
-      <c r="Y33" s="46" t="s">
+      <c r="Y33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z33" s="46"/>
+      <c r="Z33" s="48"/>
       <c r="AA33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB33" s="47"/>
-      <c r="AC33" s="48" t="s">
+      <c r="AC33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD33" s="48"/>
+      <c r="AD33" s="46"/>
       <c r="AE33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF33" s="50"/>
-      <c r="AG33" s="46" t="s">
+      <c r="AG33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH33" s="46"/>
+      <c r="AH33" s="48"/>
       <c r="AI33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ33" s="47"/>
-      <c r="AK33" s="48" t="s">
+      <c r="AK33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL33" s="48"/>
+      <c r="AL33" s="46"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J34" s="8" t="s">
@@ -5071,13 +5032,13 @@
       </c>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="51"/>
       <c r="I35">
         <v>0</v>
       </c>
@@ -5177,7 +5138,7 @@
       </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B36" s="49"/>
+      <c r="B36" s="51"/>
       <c r="C36" t="s">
         <v>39</v>
       </c>
@@ -6484,48 +6445,48 @@
       <c r="J51" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K51" s="48" t="s">
+      <c r="K51" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="46" t="s">
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="46"/>
+      <c r="O51" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P51" s="46"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="46"/>
-      <c r="S51" s="48" t="s">
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
+      <c r="R51" s="48"/>
+      <c r="S51" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T51" s="48"/>
-      <c r="U51" s="48"/>
-      <c r="V51" s="48"/>
-      <c r="W51" s="46" t="s">
+      <c r="T51" s="46"/>
+      <c r="U51" s="46"/>
+      <c r="V51" s="46"/>
+      <c r="W51" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X51" s="46"/>
-      <c r="Y51" s="46"/>
-      <c r="Z51" s="46"/>
-      <c r="AA51" s="48" t="s">
+      <c r="X51" s="48"/>
+      <c r="Y51" s="48"/>
+      <c r="Z51" s="48"/>
+      <c r="AA51" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB51" s="48"/>
-      <c r="AC51" s="48"/>
-      <c r="AD51" s="48"/>
-      <c r="AE51" s="46" t="s">
+      <c r="AB51" s="46"/>
+      <c r="AC51" s="46"/>
+      <c r="AD51" s="46"/>
+      <c r="AE51" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF51" s="46"/>
-      <c r="AG51" s="46"/>
-      <c r="AH51" s="46"/>
-      <c r="AI51" s="48" t="s">
+      <c r="AF51" s="48"/>
+      <c r="AG51" s="48"/>
+      <c r="AH51" s="48"/>
+      <c r="AI51" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ51" s="48"/>
-      <c r="AK51" s="48"/>
-      <c r="AL51" s="48"/>
+      <c r="AJ51" s="46"/>
+      <c r="AK51" s="46"/>
+      <c r="AL51" s="46"/>
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
@@ -6538,58 +6499,58 @@
         <v>41</v>
       </c>
       <c r="L52" s="47"/>
-      <c r="M52" s="51" t="s">
+      <c r="M52" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N52" s="51"/>
+      <c r="N52" s="49"/>
       <c r="O52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P52" s="50"/>
-      <c r="Q52" s="46" t="s">
+      <c r="Q52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R52" s="46"/>
+      <c r="R52" s="48"/>
       <c r="S52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T52" s="47"/>
-      <c r="U52" s="48" t="s">
+      <c r="U52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V52" s="48"/>
+      <c r="V52" s="46"/>
       <c r="W52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X52" s="50"/>
-      <c r="Y52" s="46" t="s">
+      <c r="Y52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z52" s="46"/>
+      <c r="Z52" s="48"/>
       <c r="AA52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB52" s="47"/>
-      <c r="AC52" s="48" t="s">
+      <c r="AC52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD52" s="48"/>
+      <c r="AD52" s="46"/>
       <c r="AE52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF52" s="50"/>
-      <c r="AG52" s="46" t="s">
+      <c r="AG52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH52" s="46"/>
+      <c r="AH52" s="48"/>
       <c r="AI52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ52" s="47"/>
-      <c r="AK52" s="48" t="s">
+      <c r="AK52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL52" s="48"/>
+      <c r="AL52" s="46"/>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J53" s="8" t="s">
@@ -6681,13 +6642,13 @@
       </c>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B54" s="49" t="s">
+      <c r="B54" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="49" t="s">
+      <c r="C54" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="49"/>
+      <c r="D54" s="51"/>
       <c r="I54">
         <v>0</v>
       </c>
@@ -6787,7 +6748,7 @@
       </c>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B55" s="49"/>
+      <c r="B55" s="51"/>
       <c r="C55" t="s">
         <v>39</v>
       </c>
@@ -8094,48 +8055,48 @@
       <c r="J70" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K70" s="48" t="s">
+      <c r="K70" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L70" s="48"/>
-      <c r="M70" s="48"/>
-      <c r="N70" s="48"/>
-      <c r="O70" s="46" t="s">
+      <c r="L70" s="46"/>
+      <c r="M70" s="46"/>
+      <c r="N70" s="46"/>
+      <c r="O70" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P70" s="46"/>
-      <c r="Q70" s="46"/>
-      <c r="R70" s="46"/>
-      <c r="S70" s="48" t="s">
+      <c r="P70" s="48"/>
+      <c r="Q70" s="48"/>
+      <c r="R70" s="48"/>
+      <c r="S70" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T70" s="48"/>
-      <c r="U70" s="48"/>
-      <c r="V70" s="48"/>
-      <c r="W70" s="46" t="s">
+      <c r="T70" s="46"/>
+      <c r="U70" s="46"/>
+      <c r="V70" s="46"/>
+      <c r="W70" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X70" s="46"/>
-      <c r="Y70" s="46"/>
-      <c r="Z70" s="46"/>
-      <c r="AA70" s="48" t="s">
+      <c r="X70" s="48"/>
+      <c r="Y70" s="48"/>
+      <c r="Z70" s="48"/>
+      <c r="AA70" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB70" s="48"/>
-      <c r="AC70" s="48"/>
-      <c r="AD70" s="48"/>
-      <c r="AE70" s="46" t="s">
+      <c r="AB70" s="46"/>
+      <c r="AC70" s="46"/>
+      <c r="AD70" s="46"/>
+      <c r="AE70" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF70" s="46"/>
-      <c r="AG70" s="46"/>
-      <c r="AH70" s="46"/>
-      <c r="AI70" s="48" t="s">
+      <c r="AF70" s="48"/>
+      <c r="AG70" s="48"/>
+      <c r="AH70" s="48"/>
+      <c r="AI70" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ70" s="48"/>
-      <c r="AK70" s="48"/>
-      <c r="AL70" s="48"/>
+      <c r="AJ70" s="46"/>
+      <c r="AK70" s="46"/>
+      <c r="AL70" s="46"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
@@ -8148,58 +8109,58 @@
         <v>41</v>
       </c>
       <c r="L71" s="47"/>
-      <c r="M71" s="51" t="s">
+      <c r="M71" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N71" s="51"/>
+      <c r="N71" s="49"/>
       <c r="O71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P71" s="50"/>
-      <c r="Q71" s="46" t="s">
+      <c r="Q71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R71" s="46"/>
+      <c r="R71" s="48"/>
       <c r="S71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T71" s="47"/>
-      <c r="U71" s="48" t="s">
+      <c r="U71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V71" s="48"/>
+      <c r="V71" s="46"/>
       <c r="W71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X71" s="50"/>
-      <c r="Y71" s="46" t="s">
+      <c r="Y71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z71" s="46"/>
+      <c r="Z71" s="48"/>
       <c r="AA71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB71" s="47"/>
-      <c r="AC71" s="48" t="s">
+      <c r="AC71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD71" s="48"/>
+      <c r="AD71" s="46"/>
       <c r="AE71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF71" s="50"/>
-      <c r="AG71" s="46" t="s">
+      <c r="AG71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH71" s="46"/>
+      <c r="AH71" s="48"/>
       <c r="AI71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ71" s="47"/>
-      <c r="AK71" s="48" t="s">
+      <c r="AK71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL71" s="48"/>
+      <c r="AL71" s="46"/>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J72" s="8" t="s">
@@ -8291,13 +8252,13 @@
       </c>
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B73" s="49" t="s">
+      <c r="B73" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="49" t="s">
+      <c r="C73" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="49"/>
+      <c r="D73" s="51"/>
       <c r="I73">
         <v>0</v>
       </c>
@@ -8397,7 +8358,7 @@
       </c>
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B74" s="49"/>
+      <c r="B74" s="51"/>
       <c r="C74" t="s">
         <v>39</v>
       </c>
@@ -9699,6 +9660,82 @@
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="AG71:AH71"/>
+    <mergeCell ref="AI71:AJ71"/>
+    <mergeCell ref="AK71:AL71"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="U71:V71"/>
+    <mergeCell ref="W71:X71"/>
+    <mergeCell ref="Y71:Z71"/>
+    <mergeCell ref="AA71:AB71"/>
+    <mergeCell ref="AC71:AD71"/>
+    <mergeCell ref="AE71:AF71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="S71:T71"/>
+    <mergeCell ref="S70:V70"/>
+    <mergeCell ref="W70:Z70"/>
+    <mergeCell ref="AA70:AD70"/>
+    <mergeCell ref="AE70:AH70"/>
+    <mergeCell ref="AI70:AL70"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="O70:R70"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AC52:AD52"/>
+    <mergeCell ref="AE52:AF52"/>
+    <mergeCell ref="AG52:AH52"/>
+    <mergeCell ref="AI52:AJ52"/>
+    <mergeCell ref="AK52:AL52"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="W52:X52"/>
+    <mergeCell ref="AE14:AH14"/>
+    <mergeCell ref="AI14:AL14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="W14:Z14"/>
+    <mergeCell ref="AA14:AD14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="Y52:Z52"/>
+    <mergeCell ref="AA52:AB52"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="S51:V51"/>
+    <mergeCell ref="W51:Z51"/>
+    <mergeCell ref="AA51:AD51"/>
+    <mergeCell ref="AE51:AH51"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AE33:AF33"/>
     <mergeCell ref="AC15:AD15"/>
     <mergeCell ref="AI33:AJ33"/>
     <mergeCell ref="AE32:AH32"/>
@@ -9715,82 +9752,6 @@
     <mergeCell ref="S32:V32"/>
     <mergeCell ref="W32:Z32"/>
     <mergeCell ref="AA32:AD32"/>
-    <mergeCell ref="AE51:AH51"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AE33:AF33"/>
-    <mergeCell ref="Y52:Z52"/>
-    <mergeCell ref="AA52:AB52"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="O51:R51"/>
-    <mergeCell ref="S51:V51"/>
-    <mergeCell ref="W51:Z51"/>
-    <mergeCell ref="AA51:AD51"/>
-    <mergeCell ref="AE14:AH14"/>
-    <mergeCell ref="AI14:AL14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W14:Z14"/>
-    <mergeCell ref="AA14:AD14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="O70:R70"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AC52:AD52"/>
-    <mergeCell ref="AE52:AF52"/>
-    <mergeCell ref="AG52:AH52"/>
-    <mergeCell ref="AI52:AJ52"/>
-    <mergeCell ref="AK52:AL52"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="W52:X52"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="S70:V70"/>
-    <mergeCell ref="W70:Z70"/>
-    <mergeCell ref="AA70:AD70"/>
-    <mergeCell ref="AE70:AH70"/>
-    <mergeCell ref="AI70:AL70"/>
-    <mergeCell ref="AG71:AH71"/>
-    <mergeCell ref="AI71:AJ71"/>
-    <mergeCell ref="AK71:AL71"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="U71:V71"/>
-    <mergeCell ref="W71:X71"/>
-    <mergeCell ref="Y71:Z71"/>
-    <mergeCell ref="AA71:AB71"/>
-    <mergeCell ref="AC71:AD71"/>
-    <mergeCell ref="AE71:AF71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="M71:N71"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="Q71:R71"/>
-    <mergeCell ref="S71:T71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9801,8 +9762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH171"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH36" sqref="AH36"/>
+    <sheetView topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH57" sqref="AH57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9841,137 +9802,137 @@
         <v>67</v>
       </c>
       <c r="M1" s="59"/>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="46" t="s">
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="52" t="s">
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="46" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="52" t="s">
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="46" t="s">
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="52" t="s">
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
+      <c r="AG1" s="60"/>
+      <c r="AH1" s="60"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="58" t="s">
         <v>65</v>
       </c>
       <c r="M2" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="P2" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="Q2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="57" t="s">
+      <c r="R2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="S2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="53" t="s">
+      <c r="T2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="55" t="s">
+      <c r="V2" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="57" t="s">
+      <c r="X2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="58" t="s">
+      <c r="Y2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="54" t="s">
+      <c r="AA2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="55" t="s">
+      <c r="AB2" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="56" t="s">
+      <c r="AC2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AD2" s="57" t="s">
+      <c r="AD2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AE2" s="58" t="s">
+      <c r="AE2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="AF2" s="53" t="s">
+      <c r="AF2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AH2" s="55" t="s">
+      <c r="AH2" s="54" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L3" s="60"/>
+      <c r="L3" s="58"/>
       <c r="M3" s="59"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="58"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="55"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="54"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="K4">
@@ -11337,41 +11298,41 @@
         <v>67</v>
       </c>
       <c r="M21" s="59"/>
-      <c r="N21" s="52" t="s">
+      <c r="N21" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="O21" s="52"/>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="46" t="s">
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
-      <c r="T21" s="52" t="s">
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="U21" s="52"/>
-      <c r="V21" s="52"/>
-      <c r="W21" s="46" t="s">
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X21" s="46"/>
-      <c r="Y21" s="46"/>
-      <c r="Z21" s="52" t="s">
+      <c r="X21" s="48"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AA21" s="52"/>
-      <c r="AB21" s="52"/>
-      <c r="AC21" s="46" t="s">
+      <c r="AA21" s="60"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD21" s="46"/>
-      <c r="AE21" s="46"/>
-      <c r="AF21" s="52" t="s">
+      <c r="AD21" s="48"/>
+      <c r="AE21" s="48"/>
+      <c r="AF21" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AG21" s="52"/>
-      <c r="AH21" s="52"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="60"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -11395,73 +11356,73 @@
         <f t="shared" si="1"/>
         <v>649.29999999999995</v>
       </c>
-      <c r="L22" s="60" t="s">
+      <c r="L22" s="58" t="s">
         <v>65</v>
       </c>
       <c r="M22" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="53" t="s">
+      <c r="N22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="O22" s="54" t="s">
+      <c r="O22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="P22" s="55" t="s">
+      <c r="P22" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Q22" s="56" t="s">
+      <c r="Q22" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="R22" s="57" t="s">
+      <c r="R22" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="S22" s="58" t="s">
+      <c r="S22" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T22" s="53" t="s">
+      <c r="T22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U22" s="54" t="s">
+      <c r="U22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="V22" s="55" t="s">
+      <c r="V22" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="W22" s="56" t="s">
+      <c r="W22" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X22" s="57" t="s">
+      <c r="X22" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="Y22" s="58" t="s">
+      <c r="Y22" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="Z22" s="53" t="s">
+      <c r="Z22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AA22" s="54" t="s">
+      <c r="AA22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AB22" s="55" t="s">
+      <c r="AB22" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="AC22" s="56" t="s">
+      <c r="AC22" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AD22" s="57" t="s">
+      <c r="AD22" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AE22" s="58" t="s">
+      <c r="AE22" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="AF22" s="53" t="s">
+      <c r="AF22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AG22" s="54" t="s">
+      <c r="AG22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AH22" s="55" t="s">
+      <c r="AH22" s="54" t="s">
         <v>68</v>
       </c>
     </row>
@@ -11487,29 +11448,29 @@
         <f t="shared" si="1"/>
         <v>665.8</v>
       </c>
-      <c r="L23" s="60"/>
+      <c r="L23" s="58"/>
       <c r="M23" s="59"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="55"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="57"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="55"/>
-      <c r="AC23" s="56"/>
-      <c r="AD23" s="57"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="53"/>
-      <c r="AG23" s="54"/>
-      <c r="AH23" s="55"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="57"/>
+      <c r="Z23" s="52"/>
+      <c r="AA23" s="53"/>
+      <c r="AB23" s="54"/>
+      <c r="AC23" s="55"/>
+      <c r="AD23" s="56"/>
+      <c r="AE23" s="57"/>
+      <c r="AF23" s="52"/>
+      <c r="AG23" s="53"/>
+      <c r="AH23" s="54"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -12882,41 +12843,41 @@
         <v>67</v>
       </c>
       <c r="M42" s="59"/>
-      <c r="N42" s="52" t="s">
+      <c r="N42" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="46" t="s">
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="R42" s="46"/>
-      <c r="S42" s="46"/>
-      <c r="T42" s="52" t="s">
+      <c r="R42" s="48"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="46" t="s">
+      <c r="U42" s="60"/>
+      <c r="V42" s="60"/>
+      <c r="W42" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X42" s="46"/>
-      <c r="Y42" s="46"/>
-      <c r="Z42" s="52" t="s">
+      <c r="X42" s="48"/>
+      <c r="Y42" s="48"/>
+      <c r="Z42" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AA42" s="52"/>
-      <c r="AB42" s="52"/>
-      <c r="AC42" s="46" t="s">
+      <c r="AA42" s="60"/>
+      <c r="AB42" s="60"/>
+      <c r="AC42" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD42" s="46"/>
-      <c r="AE42" s="46"/>
-      <c r="AF42" s="52" t="s">
+      <c r="AD42" s="48"/>
+      <c r="AE42" s="48"/>
+      <c r="AF42" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AG42" s="52"/>
-      <c r="AH42" s="52"/>
+      <c r="AG42" s="60"/>
+      <c r="AH42" s="60"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -12940,73 +12901,73 @@
         <f t="shared" si="1"/>
         <v>1005.61</v>
       </c>
-      <c r="L43" s="60" t="s">
+      <c r="L43" s="58" t="s">
         <v>65</v>
       </c>
       <c r="M43" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N43" s="53" t="s">
+      <c r="N43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="54" t="s">
+      <c r="O43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="P43" s="55" t="s">
+      <c r="P43" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Q43" s="56" t="s">
+      <c r="Q43" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="R43" s="57" t="s">
+      <c r="R43" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="S43" s="58" t="s">
+      <c r="S43" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T43" s="53" t="s">
+      <c r="T43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U43" s="54" t="s">
+      <c r="U43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="V43" s="55" t="s">
+      <c r="V43" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="W43" s="56" t="s">
+      <c r="W43" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X43" s="57" t="s">
+      <c r="X43" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="Y43" s="58" t="s">
+      <c r="Y43" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="Z43" s="53" t="s">
+      <c r="Z43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AA43" s="54" t="s">
+      <c r="AA43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AB43" s="55" t="s">
+      <c r="AB43" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="AC43" s="56" t="s">
+      <c r="AC43" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AD43" s="57" t="s">
+      <c r="AD43" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AE43" s="58" t="s">
+      <c r="AE43" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="AF43" s="53" t="s">
+      <c r="AF43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AG43" s="54" t="s">
+      <c r="AG43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AH43" s="55" t="s">
+      <c r="AH43" s="54" t="s">
         <v>68</v>
       </c>
     </row>
@@ -13032,29 +12993,29 @@
         <f t="shared" si="1"/>
         <v>1050.77</v>
       </c>
-      <c r="L44" s="60"/>
+      <c r="L44" s="58"/>
       <c r="M44" s="59"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="54"/>
-      <c r="P44" s="55"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="53"/>
-      <c r="U44" s="54"/>
-      <c r="V44" s="55"/>
-      <c r="W44" s="56"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="58"/>
-      <c r="Z44" s="53"/>
-      <c r="AA44" s="54"/>
-      <c r="AB44" s="55"/>
-      <c r="AC44" s="56"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="58"/>
-      <c r="AF44" s="53"/>
-      <c r="AG44" s="54"/>
-      <c r="AH44" s="55"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="55"/>
+      <c r="R44" s="56"/>
+      <c r="S44" s="57"/>
+      <c r="T44" s="52"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="54"/>
+      <c r="W44" s="55"/>
+      <c r="X44" s="56"/>
+      <c r="Y44" s="57"/>
+      <c r="Z44" s="52"/>
+      <c r="AA44" s="53"/>
+      <c r="AB44" s="54"/>
+      <c r="AC44" s="55"/>
+      <c r="AD44" s="56"/>
+      <c r="AE44" s="57"/>
+      <c r="AF44" s="52"/>
+      <c r="AG44" s="53"/>
+      <c r="AH44" s="54"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -15064,29 +15025,60 @@
     <sortCondition ref="C5:C48"/>
   </sortState>
   <mergeCells count="93">
-    <mergeCell ref="AF43:AF44"/>
-    <mergeCell ref="AG43:AG44"/>
-    <mergeCell ref="AH43:AH44"/>
-    <mergeCell ref="AA43:AA44"/>
-    <mergeCell ref="AB43:AB44"/>
-    <mergeCell ref="AC43:AC44"/>
-    <mergeCell ref="AD43:AD44"/>
-    <mergeCell ref="AE43:AE44"/>
-    <mergeCell ref="V43:V44"/>
-    <mergeCell ref="W43:W44"/>
-    <mergeCell ref="X43:X44"/>
-    <mergeCell ref="Y43:Y44"/>
-    <mergeCell ref="Z43:Z44"/>
-    <mergeCell ref="Q43:Q44"/>
-    <mergeCell ref="R43:R44"/>
-    <mergeCell ref="S43:S44"/>
-    <mergeCell ref="T43:T44"/>
-    <mergeCell ref="U43:U44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="Z21:AB21"/>
+    <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="AF21:AH21"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="V22:V23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="Z22:Z23"/>
     <mergeCell ref="AF22:AF23"/>
     <mergeCell ref="AG22:AG23"/>
     <mergeCell ref="AH22:AH23"/>
@@ -15103,60 +15095,29 @@
     <mergeCell ref="AC22:AC23"/>
     <mergeCell ref="AD22:AD23"/>
     <mergeCell ref="AE22:AE23"/>
-    <mergeCell ref="AF21:AH21"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="V22:V23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="Y22:Y23"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:Y21"/>
-    <mergeCell ref="Z21:AB21"/>
-    <mergeCell ref="AC21:AE21"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="Q43:Q44"/>
+    <mergeCell ref="R43:R44"/>
+    <mergeCell ref="S43:S44"/>
+    <mergeCell ref="T43:T44"/>
+    <mergeCell ref="U43:U44"/>
+    <mergeCell ref="V43:V44"/>
+    <mergeCell ref="W43:W44"/>
+    <mergeCell ref="X43:X44"/>
+    <mergeCell ref="Y43:Y44"/>
+    <mergeCell ref="Z43:Z44"/>
+    <mergeCell ref="AF43:AF44"/>
+    <mergeCell ref="AG43:AG44"/>
+    <mergeCell ref="AH43:AH44"/>
+    <mergeCell ref="AA43:AA44"/>
+    <mergeCell ref="AB43:AB44"/>
+    <mergeCell ref="AC43:AC44"/>
+    <mergeCell ref="AD43:AD44"/>
+    <mergeCell ref="AE43:AE44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15545,8 +15506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AL119"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D94" sqref="A88:D94"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15561,48 +15522,48 @@
       <c r="J4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="46" t="s">
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="48" t="s">
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="48"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="48"/>
-      <c r="W4" s="46" t="s">
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="48" t="s">
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="48"/>
-      <c r="AC4" s="48"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="46" t="s">
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF4" s="46"/>
-      <c r="AG4" s="46"/>
-      <c r="AH4" s="46"/>
-      <c r="AI4" s="48" t="s">
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="48"/>
-      <c r="AL4" s="48"/>
+      <c r="AJ4" s="46"/>
+      <c r="AK4" s="46"/>
+      <c r="AL4" s="46"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
@@ -15615,58 +15576,58 @@
         <v>41</v>
       </c>
       <c r="L5" s="47"/>
-      <c r="M5" s="51" t="s">
+      <c r="M5" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="51"/>
+      <c r="N5" s="49"/>
       <c r="O5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P5" s="50"/>
-      <c r="Q5" s="46" t="s">
+      <c r="Q5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="46"/>
+      <c r="R5" s="48"/>
       <c r="S5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T5" s="47"/>
-      <c r="U5" s="48" t="s">
+      <c r="U5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V5" s="48"/>
+      <c r="V5" s="46"/>
       <c r="W5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X5" s="50"/>
-      <c r="Y5" s="46" t="s">
+      <c r="Y5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="46"/>
+      <c r="Z5" s="48"/>
       <c r="AA5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB5" s="47"/>
-      <c r="AC5" s="48" t="s">
+      <c r="AC5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD5" s="48"/>
+      <c r="AD5" s="46"/>
       <c r="AE5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF5" s="50"/>
-      <c r="AG5" s="46" t="s">
+      <c r="AG5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH5" s="46"/>
+      <c r="AH5" s="48"/>
       <c r="AI5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ5" s="47"/>
-      <c r="AK5" s="48" t="s">
+      <c r="AK5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL5" s="48"/>
+      <c r="AL5" s="46"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J6" s="8" t="s">
@@ -15758,13 +15719,13 @@
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="51"/>
       <c r="I7">
         <v>0</v>
       </c>
@@ -15864,7 +15825,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="51"/>
       <c r="C8" t="s">
         <v>39</v>
       </c>
@@ -19011,48 +18972,48 @@
       <c r="J43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K43" s="48" t="s">
+      <c r="K43" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="46" t="s">
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P43" s="46"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="46"/>
-      <c r="S43" s="48" t="s">
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-      <c r="V43" s="48"/>
-      <c r="W43" s="46" t="s">
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X43" s="46"/>
-      <c r="Y43" s="46"/>
-      <c r="Z43" s="46"/>
-      <c r="AA43" s="48" t="s">
+      <c r="X43" s="48"/>
+      <c r="Y43" s="48"/>
+      <c r="Z43" s="48"/>
+      <c r="AA43" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB43" s="48"/>
-      <c r="AC43" s="48"/>
-      <c r="AD43" s="48"/>
-      <c r="AE43" s="46" t="s">
+      <c r="AB43" s="46"/>
+      <c r="AC43" s="46"/>
+      <c r="AD43" s="46"/>
+      <c r="AE43" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF43" s="46"/>
-      <c r="AG43" s="46"/>
-      <c r="AH43" s="46"/>
-      <c r="AI43" s="48" t="s">
+      <c r="AF43" s="48"/>
+      <c r="AG43" s="48"/>
+      <c r="AH43" s="48"/>
+      <c r="AI43" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ43" s="48"/>
-      <c r="AK43" s="48"/>
-      <c r="AL43" s="48"/>
+      <c r="AJ43" s="46"/>
+      <c r="AK43" s="46"/>
+      <c r="AL43" s="46"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
@@ -19065,58 +19026,58 @@
         <v>41</v>
       </c>
       <c r="L44" s="47"/>
-      <c r="M44" s="51" t="s">
+      <c r="M44" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N44" s="51"/>
+      <c r="N44" s="49"/>
       <c r="O44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P44" s="50"/>
-      <c r="Q44" s="46" t="s">
+      <c r="Q44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R44" s="46"/>
+      <c r="R44" s="48"/>
       <c r="S44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T44" s="47"/>
-      <c r="U44" s="48" t="s">
+      <c r="U44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V44" s="48"/>
+      <c r="V44" s="46"/>
       <c r="W44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X44" s="50"/>
-      <c r="Y44" s="46" t="s">
+      <c r="Y44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z44" s="46"/>
+      <c r="Z44" s="48"/>
       <c r="AA44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB44" s="47"/>
-      <c r="AC44" s="48" t="s">
+      <c r="AC44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD44" s="48"/>
+      <c r="AD44" s="46"/>
       <c r="AE44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF44" s="50"/>
-      <c r="AG44" s="46" t="s">
+      <c r="AG44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH44" s="46"/>
+      <c r="AH44" s="48"/>
       <c r="AI44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ44" s="47"/>
-      <c r="AK44" s="48" t="s">
+      <c r="AK44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL44" s="48"/>
+      <c r="AL44" s="46"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J45" s="8" t="s">
@@ -19208,13 +19169,13 @@
       </c>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="49" t="s">
+      <c r="C46" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="49"/>
+      <c r="D46" s="51"/>
       <c r="I46">
         <v>0</v>
       </c>
@@ -19314,7 +19275,7 @@
       </c>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B47" s="49"/>
+      <c r="B47" s="51"/>
       <c r="C47" t="s">
         <v>39</v>
       </c>
@@ -22369,48 +22330,48 @@
       <c r="J83" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K83" s="48" t="s">
+      <c r="K83" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L83" s="48"/>
-      <c r="M83" s="48"/>
-      <c r="N83" s="48"/>
-      <c r="O83" s="46" t="s">
+      <c r="L83" s="46"/>
+      <c r="M83" s="46"/>
+      <c r="N83" s="46"/>
+      <c r="O83" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P83" s="46"/>
-      <c r="Q83" s="46"/>
-      <c r="R83" s="46"/>
-      <c r="S83" s="48" t="s">
+      <c r="P83" s="48"/>
+      <c r="Q83" s="48"/>
+      <c r="R83" s="48"/>
+      <c r="S83" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T83" s="48"/>
-      <c r="U83" s="48"/>
-      <c r="V83" s="48"/>
-      <c r="W83" s="46" t="s">
+      <c r="T83" s="46"/>
+      <c r="U83" s="46"/>
+      <c r="V83" s="46"/>
+      <c r="W83" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X83" s="46"/>
-      <c r="Y83" s="46"/>
-      <c r="Z83" s="46"/>
-      <c r="AA83" s="48" t="s">
+      <c r="X83" s="48"/>
+      <c r="Y83" s="48"/>
+      <c r="Z83" s="48"/>
+      <c r="AA83" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB83" s="48"/>
-      <c r="AC83" s="48"/>
-      <c r="AD83" s="48"/>
-      <c r="AE83" s="46" t="s">
+      <c r="AB83" s="46"/>
+      <c r="AC83" s="46"/>
+      <c r="AD83" s="46"/>
+      <c r="AE83" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF83" s="46"/>
-      <c r="AG83" s="46"/>
-      <c r="AH83" s="46"/>
-      <c r="AI83" s="48" t="s">
+      <c r="AF83" s="48"/>
+      <c r="AG83" s="48"/>
+      <c r="AH83" s="48"/>
+      <c r="AI83" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ83" s="48"/>
-      <c r="AK83" s="48"/>
-      <c r="AL83" s="48"/>
+      <c r="AJ83" s="46"/>
+      <c r="AK83" s="46"/>
+      <c r="AL83" s="46"/>
     </row>
     <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H84" t="s">
@@ -22423,58 +22384,58 @@
         <v>41</v>
       </c>
       <c r="L84" s="47"/>
-      <c r="M84" s="51" t="s">
+      <c r="M84" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N84" s="51"/>
+      <c r="N84" s="49"/>
       <c r="O84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P84" s="50"/>
-      <c r="Q84" s="46" t="s">
+      <c r="Q84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R84" s="46"/>
+      <c r="R84" s="48"/>
       <c r="S84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T84" s="47"/>
-      <c r="U84" s="48" t="s">
+      <c r="U84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V84" s="48"/>
+      <c r="V84" s="46"/>
       <c r="W84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X84" s="50"/>
-      <c r="Y84" s="46" t="s">
+      <c r="Y84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z84" s="46"/>
+      <c r="Z84" s="48"/>
       <c r="AA84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB84" s="47"/>
-      <c r="AC84" s="48" t="s">
+      <c r="AC84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD84" s="48"/>
+      <c r="AD84" s="46"/>
       <c r="AE84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF84" s="50"/>
-      <c r="AG84" s="46" t="s">
+      <c r="AG84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH84" s="46"/>
+      <c r="AH84" s="48"/>
       <c r="AI84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ84" s="47"/>
-      <c r="AK84" s="48" t="s">
+      <c r="AK84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL84" s="48"/>
+      <c r="AL84" s="46"/>
     </row>
     <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J85" s="8" t="s">
@@ -22566,13 +22527,13 @@
       </c>
     </row>
     <row r="86" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B86" s="49" t="s">
+      <c r="B86" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C86" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D86" s="49"/>
+      <c r="D86" s="51"/>
       <c r="I86">
         <v>0</v>
       </c>
@@ -22672,7 +22633,7 @@
       </c>
     </row>
     <row r="87" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B87" s="49"/>
+      <c r="B87" s="51"/>
       <c r="C87" t="s">
         <v>39</v>
       </c>
@@ -25726,6 +25687,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="AI84:AJ84"/>
+    <mergeCell ref="AK84:AL84"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="W83:Z83"/>
+    <mergeCell ref="AA83:AD83"/>
+    <mergeCell ref="AE83:AH83"/>
+    <mergeCell ref="AI83:AL83"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="O84:P84"/>
+    <mergeCell ref="Q84:R84"/>
+    <mergeCell ref="S84:T84"/>
+    <mergeCell ref="U84:V84"/>
+    <mergeCell ref="W84:X84"/>
+    <mergeCell ref="Y84:Z84"/>
+    <mergeCell ref="AA84:AB84"/>
+    <mergeCell ref="AC84:AD84"/>
+    <mergeCell ref="AE84:AF84"/>
+    <mergeCell ref="AG84:AH84"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="O83:R83"/>
+    <mergeCell ref="S83:V83"/>
+    <mergeCell ref="AE43:AH43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="W44:X44"/>
+    <mergeCell ref="Y44:Z44"/>
+    <mergeCell ref="AA44:AB44"/>
+    <mergeCell ref="AC44:AD44"/>
+    <mergeCell ref="AE44:AF44"/>
+    <mergeCell ref="AG44:AH44"/>
+    <mergeCell ref="AI44:AJ44"/>
+    <mergeCell ref="AK44:AL44"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="O43:R43"/>
+    <mergeCell ref="S43:V43"/>
+    <mergeCell ref="W43:Z43"/>
+    <mergeCell ref="AA43:AD43"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="AE4:AH4"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="AI4:AL4"/>
@@ -25742,59 +25756,6 @@
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="O43:R43"/>
-    <mergeCell ref="S43:V43"/>
-    <mergeCell ref="W43:Z43"/>
-    <mergeCell ref="AA43:AD43"/>
-    <mergeCell ref="AE43:AH43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="W44:X44"/>
-    <mergeCell ref="Y44:Z44"/>
-    <mergeCell ref="AA44:AB44"/>
-    <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="AE44:AF44"/>
-    <mergeCell ref="AG44:AH44"/>
-    <mergeCell ref="AI44:AJ44"/>
-    <mergeCell ref="AK44:AL44"/>
-    <mergeCell ref="AA84:AB84"/>
-    <mergeCell ref="AC84:AD84"/>
-    <mergeCell ref="AE84:AF84"/>
-    <mergeCell ref="AG84:AH84"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="O83:R83"/>
-    <mergeCell ref="S83:V83"/>
-    <mergeCell ref="AI84:AJ84"/>
-    <mergeCell ref="AK84:AL84"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="W83:Z83"/>
-    <mergeCell ref="AA83:AD83"/>
-    <mergeCell ref="AE83:AH83"/>
-    <mergeCell ref="AI83:AL83"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="O84:P84"/>
-    <mergeCell ref="Q84:R84"/>
-    <mergeCell ref="S84:T84"/>
-    <mergeCell ref="U84:V84"/>
-    <mergeCell ref="W84:X84"/>
-    <mergeCell ref="Y84:Z84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25805,8 +25766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M113" sqref="M113"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35786,7 +35747,7 @@
         <v>3346.3111764705882</v>
       </c>
       <c r="N112" s="29">
-        <f t="shared" ref="M112:O112" si="36">AVERAGE(N101:N109,N91:N99,N81:N89)</f>
+        <f t="shared" ref="N112:O112" si="36">AVERAGE(N101:N109,N91:N99,N81:N89)</f>
         <v>27.944444444444443</v>
       </c>
       <c r="O112" s="27">

</xml_diff>

<commit_message>
Fix a bad copy paste in results spreadsheet
</commit_message>
<xml_diff>
--- a/Miscellaneous/results.xlsx
+++ b/Miscellaneous/results.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarog\dissertation\Miscellaneous\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-225" yWindow="-165" windowWidth="27795" windowHeight="14310" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="-225" yWindow="-165" windowWidth="27795" windowHeight="14310" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meshing stuff" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
     <sheet name="3D Subray" sheetId="7" r:id="rId7"/>
     <sheet name="3D Subray Runtime" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -466,7 +461,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.##\%;[Red]\(0.##\%\)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -660,25 +655,22 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -699,10 +691,13 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +763,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -801,26 +796,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -853,23 +831,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3276,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AL85"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD54" sqref="AD54:AD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3527,48 +3488,48 @@
       <c r="J14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="46" t="s">
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="48" t="s">
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="46" t="s">
+      <c r="T14" s="46"/>
+      <c r="U14" s="46"/>
+      <c r="V14" s="46"/>
+      <c r="W14" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="48" t="s">
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB14" s="48"/>
-      <c r="AC14" s="48"/>
-      <c r="AD14" s="48"/>
-      <c r="AE14" s="46" t="s">
+      <c r="AB14" s="46"/>
+      <c r="AC14" s="46"/>
+      <c r="AD14" s="46"/>
+      <c r="AE14" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF14" s="46"/>
-      <c r="AG14" s="46"/>
-      <c r="AH14" s="46"/>
-      <c r="AI14" s="48" t="s">
+      <c r="AF14" s="48"/>
+      <c r="AG14" s="48"/>
+      <c r="AH14" s="48"/>
+      <c r="AI14" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ14" s="48"/>
-      <c r="AK14" s="48"/>
-      <c r="AL14" s="48"/>
+      <c r="AJ14" s="46"/>
+      <c r="AK14" s="46"/>
+      <c r="AL14" s="46"/>
     </row>
     <row r="15" spans="4:38" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
@@ -3581,58 +3542,58 @@
         <v>41</v>
       </c>
       <c r="L15" s="47"/>
-      <c r="M15" s="51" t="s">
+      <c r="M15" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="51"/>
+      <c r="N15" s="49"/>
       <c r="O15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P15" s="50"/>
-      <c r="Q15" s="46" t="s">
+      <c r="Q15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="46"/>
+      <c r="R15" s="48"/>
       <c r="S15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T15" s="47"/>
-      <c r="U15" s="48" t="s">
+      <c r="U15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V15" s="48"/>
+      <c r="V15" s="46"/>
       <c r="W15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X15" s="50"/>
-      <c r="Y15" s="46" t="s">
+      <c r="Y15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z15" s="46"/>
+      <c r="Z15" s="48"/>
       <c r="AA15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB15" s="47"/>
-      <c r="AC15" s="48" t="s">
+      <c r="AC15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD15" s="48"/>
+      <c r="AD15" s="46"/>
       <c r="AE15" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF15" s="50"/>
-      <c r="AG15" s="46" t="s">
+      <c r="AG15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH15" s="46"/>
+      <c r="AH15" s="48"/>
       <c r="AI15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ15" s="47"/>
-      <c r="AK15" s="48" t="s">
+      <c r="AK15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL15" s="48"/>
+      <c r="AL15" s="46"/>
     </row>
     <row r="16" spans="4:38" x14ac:dyDescent="0.25">
       <c r="J16" s="8" t="s">
@@ -3724,13 +3685,13 @@
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="51"/>
       <c r="I17">
         <v>0</v>
       </c>
@@ -3785,7 +3746,7 @@
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B18" s="49"/>
+      <c r="B18" s="51"/>
       <c r="C18" t="s">
         <v>39</v>
       </c>
@@ -4802,48 +4763,48 @@
       <c r="J32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="48" t="s">
+      <c r="K32" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="46" t="s">
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="48" t="s">
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T32" s="48"/>
-      <c r="U32" s="48"/>
-      <c r="V32" s="48"/>
-      <c r="W32" s="46" t="s">
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X32" s="46"/>
-      <c r="Y32" s="46"/>
-      <c r="Z32" s="46"/>
-      <c r="AA32" s="48" t="s">
+      <c r="X32" s="48"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="48"/>
+      <c r="AA32" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB32" s="48"/>
-      <c r="AC32" s="48"/>
-      <c r="AD32" s="48"/>
-      <c r="AE32" s="46" t="s">
+      <c r="AB32" s="46"/>
+      <c r="AC32" s="46"/>
+      <c r="AD32" s="46"/>
+      <c r="AE32" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF32" s="46"/>
-      <c r="AG32" s="46"/>
-      <c r="AH32" s="46"/>
-      <c r="AI32" s="48" t="s">
+      <c r="AF32" s="48"/>
+      <c r="AG32" s="48"/>
+      <c r="AH32" s="48"/>
+      <c r="AI32" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ32" s="48"/>
-      <c r="AK32" s="48"/>
-      <c r="AL32" s="48"/>
+      <c r="AJ32" s="46"/>
+      <c r="AK32" s="46"/>
+      <c r="AL32" s="46"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
@@ -4856,58 +4817,58 @@
         <v>41</v>
       </c>
       <c r="L33" s="47"/>
-      <c r="M33" s="51" t="s">
+      <c r="M33" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N33" s="51"/>
+      <c r="N33" s="49"/>
       <c r="O33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P33" s="50"/>
-      <c r="Q33" s="46" t="s">
+      <c r="Q33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R33" s="46"/>
+      <c r="R33" s="48"/>
       <c r="S33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T33" s="47"/>
-      <c r="U33" s="48" t="s">
+      <c r="U33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V33" s="48"/>
+      <c r="V33" s="46"/>
       <c r="W33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X33" s="50"/>
-      <c r="Y33" s="46" t="s">
+      <c r="Y33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z33" s="46"/>
+      <c r="Z33" s="48"/>
       <c r="AA33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB33" s="47"/>
-      <c r="AC33" s="48" t="s">
+      <c r="AC33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD33" s="48"/>
+      <c r="AD33" s="46"/>
       <c r="AE33" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF33" s="50"/>
-      <c r="AG33" s="46" t="s">
+      <c r="AG33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH33" s="46"/>
+      <c r="AH33" s="48"/>
       <c r="AI33" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ33" s="47"/>
-      <c r="AK33" s="48" t="s">
+      <c r="AK33" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL33" s="48"/>
+      <c r="AL33" s="46"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J34" s="8" t="s">
@@ -4999,13 +4960,13 @@
       </c>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="51"/>
       <c r="I35">
         <v>0</v>
       </c>
@@ -5105,7 +5066,7 @@
       </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B36" s="49"/>
+      <c r="B36" s="51"/>
       <c r="C36" t="s">
         <v>39</v>
       </c>
@@ -6412,48 +6373,48 @@
       <c r="J51" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K51" s="48" t="s">
+      <c r="K51" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="46" t="s">
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="46"/>
+      <c r="O51" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P51" s="46"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="46"/>
-      <c r="S51" s="48" t="s">
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
+      <c r="R51" s="48"/>
+      <c r="S51" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T51" s="48"/>
-      <c r="U51" s="48"/>
-      <c r="V51" s="48"/>
-      <c r="W51" s="46" t="s">
+      <c r="T51" s="46"/>
+      <c r="U51" s="46"/>
+      <c r="V51" s="46"/>
+      <c r="W51" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X51" s="46"/>
-      <c r="Y51" s="46"/>
-      <c r="Z51" s="46"/>
-      <c r="AA51" s="48" t="s">
+      <c r="X51" s="48"/>
+      <c r="Y51" s="48"/>
+      <c r="Z51" s="48"/>
+      <c r="AA51" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB51" s="48"/>
-      <c r="AC51" s="48"/>
-      <c r="AD51" s="48"/>
-      <c r="AE51" s="46" t="s">
+      <c r="AB51" s="46"/>
+      <c r="AC51" s="46"/>
+      <c r="AD51" s="46"/>
+      <c r="AE51" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF51" s="46"/>
-      <c r="AG51" s="46"/>
-      <c r="AH51" s="46"/>
-      <c r="AI51" s="48" t="s">
+      <c r="AF51" s="48"/>
+      <c r="AG51" s="48"/>
+      <c r="AH51" s="48"/>
+      <c r="AI51" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ51" s="48"/>
-      <c r="AK51" s="48"/>
-      <c r="AL51" s="48"/>
+      <c r="AJ51" s="46"/>
+      <c r="AK51" s="46"/>
+      <c r="AL51" s="46"/>
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
@@ -6466,58 +6427,58 @@
         <v>41</v>
       </c>
       <c r="L52" s="47"/>
-      <c r="M52" s="51" t="s">
+      <c r="M52" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N52" s="51"/>
+      <c r="N52" s="49"/>
       <c r="O52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P52" s="50"/>
-      <c r="Q52" s="46" t="s">
+      <c r="Q52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R52" s="46"/>
+      <c r="R52" s="48"/>
       <c r="S52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T52" s="47"/>
-      <c r="U52" s="48" t="s">
+      <c r="U52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V52" s="48"/>
+      <c r="V52" s="46"/>
       <c r="W52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X52" s="50"/>
-      <c r="Y52" s="46" t="s">
+      <c r="Y52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z52" s="46"/>
+      <c r="Z52" s="48"/>
       <c r="AA52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB52" s="47"/>
-      <c r="AC52" s="48" t="s">
+      <c r="AC52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD52" s="48"/>
+      <c r="AD52" s="46"/>
       <c r="AE52" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF52" s="50"/>
-      <c r="AG52" s="46" t="s">
+      <c r="AG52" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH52" s="46"/>
+      <c r="AH52" s="48"/>
       <c r="AI52" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ52" s="47"/>
-      <c r="AK52" s="48" t="s">
+      <c r="AK52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL52" s="48"/>
+      <c r="AL52" s="46"/>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J53" s="8" t="s">
@@ -6609,13 +6570,13 @@
       </c>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B54" s="49" t="s">
+      <c r="B54" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="49" t="s">
+      <c r="C54" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="49"/>
+      <c r="D54" s="51"/>
       <c r="I54">
         <v>0</v>
       </c>
@@ -6685,7 +6646,7 @@
         <v>0</v>
       </c>
       <c r="AD54" s="19">
-        <v>4.4695359999999997</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AE54" s="12">
         <v>1.0623800000000001</v>
@@ -6715,7 +6676,7 @@
       </c>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B55" s="49"/>
+      <c r="B55" s="51"/>
       <c r="C55" t="s">
         <v>39</v>
       </c>
@@ -6791,7 +6752,7 @@
         <v>1.729206</v>
       </c>
       <c r="AD55" s="19">
-        <v>12.696300000000001</v>
+        <v>4.4695359999999997</v>
       </c>
       <c r="AE55" s="12">
         <v>1.067518</v>
@@ -6830,11 +6791,11 @@
       </c>
       <c r="C56" s="25">
         <f>AC65</f>
-        <v>8.6460314444444446</v>
+        <v>8.6460304444444436</v>
       </c>
       <c r="D56" s="25">
         <f>AD65</f>
-        <v>25.492478444444448</v>
+        <v>25.989083999999998</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="25"/>
@@ -6908,7 +6869,7 @@
         <v>4.7484669999999998</v>
       </c>
       <c r="AD56" s="19">
-        <v>21.297630000000002</v>
+        <v>12.696300000000001</v>
       </c>
       <c r="AE56" s="12">
         <v>1.07548</v>
@@ -7025,7 +6986,7 @@
         <v>7.7146739999999996</v>
       </c>
       <c r="AD57" s="19">
-        <v>29.418970000000002</v>
+        <v>21.297630000000002</v>
       </c>
       <c r="AE57" s="12">
         <v>1.0848690000000001</v>
@@ -7142,7 +7103,7 @@
         <v>10.326420000000001</v>
       </c>
       <c r="AD58" s="19">
-        <v>36.00215</v>
+        <v>29.418970000000002</v>
       </c>
       <c r="AE58" s="12">
         <v>1.095596</v>
@@ -7256,10 +7217,10 @@
         <v>-2399.99999999998</v>
       </c>
       <c r="AC59" s="19">
-        <v>12.246286</v>
+        <v>12.24628</v>
       </c>
       <c r="AD59" s="19">
-        <v>39.828629999999997</v>
+        <v>36.00215</v>
       </c>
       <c r="AE59" s="12">
         <v>1.1075550000000001</v>
@@ -7373,10 +7334,10 @@
         <v>-2737.7999999999902</v>
       </c>
       <c r="AC60" s="19">
-        <v>13.120651000000001</v>
+        <v>13.120649999999999</v>
       </c>
       <c r="AD60" s="19">
-        <v>39.382390000000001</v>
+        <v>39.828629999999997</v>
       </c>
       <c r="AE60" s="12">
         <v>1.120708</v>
@@ -7490,10 +7451,10 @@
         <v>-2819.599999999989</v>
       </c>
       <c r="AC61" s="19">
-        <v>12.545552000000001</v>
+        <v>12.54555</v>
       </c>
       <c r="AD61" s="19">
-        <v>32.802230000000002</v>
+        <v>39.382390000000001</v>
       </c>
       <c r="AE61" s="12">
         <v>1.135089</v>
@@ -7610,7 +7571,7 @@
         <v>10.07649</v>
       </c>
       <c r="AD62" s="19">
-        <v>18.003920000000001</v>
+        <v>32.802230000000002</v>
       </c>
       <c r="AE62" s="12">
         <v>1.1509199999999999</v>
@@ -7709,7 +7670,7 @@
         <v>5.3065369999999996</v>
       </c>
       <c r="AD63" s="19">
-        <v>8.6000000000000003E-5</v>
+        <v>18.003920000000001</v>
       </c>
       <c r="AE63" s="12">
         <v>1.1689050000000001</v>
@@ -7895,11 +7856,11 @@
       </c>
       <c r="AC65" s="19">
         <f>AVERAGE(AC55:AC63)</f>
-        <v>8.6460314444444446</v>
+        <v>8.6460304444444436</v>
       </c>
       <c r="AD65" s="19">
         <f>AVERAGE(AD55:AD63)</f>
-        <v>25.492478444444448</v>
+        <v>25.989083999999998</v>
       </c>
       <c r="AF65" s="17">
         <f t="array" ref="AF65">AVERAGE(ABS(AF55:AF63))</f>
@@ -7984,11 +7945,11 @@
       </c>
       <c r="AC66" s="19">
         <f>AVERAGE(AC56:AC62)</f>
-        <v>10.111219999999999</v>
+        <v>10.111218714285712</v>
       </c>
       <c r="AD66" s="19">
         <f>AVERAGE(AD56:AD62)</f>
-        <v>30.96227428571429</v>
+        <v>30.204042857142863</v>
       </c>
       <c r="AF66" s="17">
         <f t="array" ref="AF66">AVERAGE(ABS(AF56:AF62))</f>
@@ -8022,48 +7983,48 @@
       <c r="J70" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K70" s="48" t="s">
+      <c r="K70" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L70" s="48"/>
-      <c r="M70" s="48"/>
-      <c r="N70" s="48"/>
-      <c r="O70" s="46" t="s">
+      <c r="L70" s="46"/>
+      <c r="M70" s="46"/>
+      <c r="N70" s="46"/>
+      <c r="O70" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P70" s="46"/>
-      <c r="Q70" s="46"/>
-      <c r="R70" s="46"/>
-      <c r="S70" s="48" t="s">
+      <c r="P70" s="48"/>
+      <c r="Q70" s="48"/>
+      <c r="R70" s="48"/>
+      <c r="S70" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T70" s="48"/>
-      <c r="U70" s="48"/>
-      <c r="V70" s="48"/>
-      <c r="W70" s="46" t="s">
+      <c r="T70" s="46"/>
+      <c r="U70" s="46"/>
+      <c r="V70" s="46"/>
+      <c r="W70" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X70" s="46"/>
-      <c r="Y70" s="46"/>
-      <c r="Z70" s="46"/>
-      <c r="AA70" s="48" t="s">
+      <c r="X70" s="48"/>
+      <c r="Y70" s="48"/>
+      <c r="Z70" s="48"/>
+      <c r="AA70" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB70" s="48"/>
-      <c r="AC70" s="48"/>
-      <c r="AD70" s="48"/>
-      <c r="AE70" s="46" t="s">
+      <c r="AB70" s="46"/>
+      <c r="AC70" s="46"/>
+      <c r="AD70" s="46"/>
+      <c r="AE70" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF70" s="46"/>
-      <c r="AG70" s="46"/>
-      <c r="AH70" s="46"/>
-      <c r="AI70" s="48" t="s">
+      <c r="AF70" s="48"/>
+      <c r="AG70" s="48"/>
+      <c r="AH70" s="48"/>
+      <c r="AI70" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ70" s="48"/>
-      <c r="AK70" s="48"/>
-      <c r="AL70" s="48"/>
+      <c r="AJ70" s="46"/>
+      <c r="AK70" s="46"/>
+      <c r="AL70" s="46"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
@@ -8076,58 +8037,58 @@
         <v>41</v>
       </c>
       <c r="L71" s="47"/>
-      <c r="M71" s="51" t="s">
+      <c r="M71" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N71" s="51"/>
+      <c r="N71" s="49"/>
       <c r="O71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P71" s="50"/>
-      <c r="Q71" s="46" t="s">
+      <c r="Q71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R71" s="46"/>
+      <c r="R71" s="48"/>
       <c r="S71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T71" s="47"/>
-      <c r="U71" s="48" t="s">
+      <c r="U71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V71" s="48"/>
+      <c r="V71" s="46"/>
       <c r="W71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X71" s="50"/>
-      <c r="Y71" s="46" t="s">
+      <c r="Y71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z71" s="46"/>
+      <c r="Z71" s="48"/>
       <c r="AA71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB71" s="47"/>
-      <c r="AC71" s="48" t="s">
+      <c r="AC71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD71" s="48"/>
+      <c r="AD71" s="46"/>
       <c r="AE71" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF71" s="50"/>
-      <c r="AG71" s="46" t="s">
+      <c r="AG71" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH71" s="46"/>
+      <c r="AH71" s="48"/>
       <c r="AI71" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ71" s="47"/>
-      <c r="AK71" s="48" t="s">
+      <c r="AK71" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL71" s="48"/>
+      <c r="AL71" s="46"/>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J72" s="8" t="s">
@@ -8219,13 +8180,13 @@
       </c>
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B73" s="49" t="s">
+      <c r="B73" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="49" t="s">
+      <c r="C73" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="49"/>
+      <c r="D73" s="51"/>
       <c r="I73">
         <v>0</v>
       </c>
@@ -8325,7 +8286,7 @@
       </c>
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B74" s="49"/>
+      <c r="B74" s="51"/>
       <c r="C74" t="s">
         <v>39</v>
       </c>
@@ -9627,6 +9588,82 @@
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="AG71:AH71"/>
+    <mergeCell ref="AI71:AJ71"/>
+    <mergeCell ref="AK71:AL71"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="U71:V71"/>
+    <mergeCell ref="W71:X71"/>
+    <mergeCell ref="Y71:Z71"/>
+    <mergeCell ref="AA71:AB71"/>
+    <mergeCell ref="AC71:AD71"/>
+    <mergeCell ref="AE71:AF71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="S71:T71"/>
+    <mergeCell ref="S70:V70"/>
+    <mergeCell ref="W70:Z70"/>
+    <mergeCell ref="AA70:AD70"/>
+    <mergeCell ref="AE70:AH70"/>
+    <mergeCell ref="AI70:AL70"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="O70:R70"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AC52:AD52"/>
+    <mergeCell ref="AE52:AF52"/>
+    <mergeCell ref="AG52:AH52"/>
+    <mergeCell ref="AI52:AJ52"/>
+    <mergeCell ref="AK52:AL52"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="W52:X52"/>
+    <mergeCell ref="AE14:AH14"/>
+    <mergeCell ref="AI14:AL14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="W14:Z14"/>
+    <mergeCell ref="AA14:AD14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="Y52:Z52"/>
+    <mergeCell ref="AA52:AB52"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="S51:V51"/>
+    <mergeCell ref="W51:Z51"/>
+    <mergeCell ref="AA51:AD51"/>
+    <mergeCell ref="AE51:AH51"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AE33:AF33"/>
     <mergeCell ref="AC15:AD15"/>
     <mergeCell ref="AI33:AJ33"/>
     <mergeCell ref="AE32:AH32"/>
@@ -9643,82 +9680,6 @@
     <mergeCell ref="S32:V32"/>
     <mergeCell ref="W32:Z32"/>
     <mergeCell ref="AA32:AD32"/>
-    <mergeCell ref="AE51:AH51"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AE33:AF33"/>
-    <mergeCell ref="Y52:Z52"/>
-    <mergeCell ref="AA52:AB52"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="O51:R51"/>
-    <mergeCell ref="S51:V51"/>
-    <mergeCell ref="W51:Z51"/>
-    <mergeCell ref="AA51:AD51"/>
-    <mergeCell ref="AE14:AH14"/>
-    <mergeCell ref="AI14:AL14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W14:Z14"/>
-    <mergeCell ref="AA14:AD14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="O70:R70"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AC52:AD52"/>
-    <mergeCell ref="AE52:AF52"/>
-    <mergeCell ref="AG52:AH52"/>
-    <mergeCell ref="AI52:AJ52"/>
-    <mergeCell ref="AK52:AL52"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="W52:X52"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="S70:V70"/>
-    <mergeCell ref="W70:Z70"/>
-    <mergeCell ref="AA70:AD70"/>
-    <mergeCell ref="AE70:AH70"/>
-    <mergeCell ref="AI70:AL70"/>
-    <mergeCell ref="AG71:AH71"/>
-    <mergeCell ref="AI71:AJ71"/>
-    <mergeCell ref="AK71:AL71"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="U71:V71"/>
-    <mergeCell ref="W71:X71"/>
-    <mergeCell ref="Y71:Z71"/>
-    <mergeCell ref="AA71:AB71"/>
-    <mergeCell ref="AC71:AD71"/>
-    <mergeCell ref="AE71:AF71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="M71:N71"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="Q71:R71"/>
-    <mergeCell ref="S71:T71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9769,137 +9730,137 @@
         <v>67</v>
       </c>
       <c r="M1" s="59"/>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="46" t="s">
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="52" t="s">
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="46" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="52" t="s">
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="46" t="s">
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="52" t="s">
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
+      <c r="AG1" s="60"/>
+      <c r="AH1" s="60"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="58" t="s">
         <v>65</v>
       </c>
       <c r="M2" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="P2" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="Q2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="57" t="s">
+      <c r="R2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="S2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="53" t="s">
+      <c r="T2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="55" t="s">
+      <c r="V2" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="57" t="s">
+      <c r="X2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="58" t="s">
+      <c r="Y2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="54" t="s">
+      <c r="AA2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="55" t="s">
+      <c r="AB2" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="56" t="s">
+      <c r="AC2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AD2" s="57" t="s">
+      <c r="AD2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AE2" s="58" t="s">
+      <c r="AE2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="AF2" s="53" t="s">
+      <c r="AF2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AH2" s="55" t="s">
+      <c r="AH2" s="54" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L3" s="60"/>
+      <c r="L3" s="58"/>
       <c r="M3" s="59"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="58"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="55"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="54"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="K4">
@@ -11265,41 +11226,41 @@
         <v>67</v>
       </c>
       <c r="M21" s="59"/>
-      <c r="N21" s="52" t="s">
+      <c r="N21" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="O21" s="52"/>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="46" t="s">
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
-      <c r="T21" s="52" t="s">
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="U21" s="52"/>
-      <c r="V21" s="52"/>
-      <c r="W21" s="46" t="s">
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X21" s="46"/>
-      <c r="Y21" s="46"/>
-      <c r="Z21" s="52" t="s">
+      <c r="X21" s="48"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AA21" s="52"/>
-      <c r="AB21" s="52"/>
-      <c r="AC21" s="46" t="s">
+      <c r="AA21" s="60"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD21" s="46"/>
-      <c r="AE21" s="46"/>
-      <c r="AF21" s="52" t="s">
+      <c r="AD21" s="48"/>
+      <c r="AE21" s="48"/>
+      <c r="AF21" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AG21" s="52"/>
-      <c r="AH21" s="52"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="60"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -11323,73 +11284,73 @@
         <f t="shared" si="1"/>
         <v>649.29999999999995</v>
       </c>
-      <c r="L22" s="60" t="s">
+      <c r="L22" s="58" t="s">
         <v>65</v>
       </c>
       <c r="M22" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="53" t="s">
+      <c r="N22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="O22" s="54" t="s">
+      <c r="O22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="P22" s="55" t="s">
+      <c r="P22" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Q22" s="56" t="s">
+      <c r="Q22" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="R22" s="57" t="s">
+      <c r="R22" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="S22" s="58" t="s">
+      <c r="S22" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T22" s="53" t="s">
+      <c r="T22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U22" s="54" t="s">
+      <c r="U22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="V22" s="55" t="s">
+      <c r="V22" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="W22" s="56" t="s">
+      <c r="W22" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X22" s="57" t="s">
+      <c r="X22" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="Y22" s="58" t="s">
+      <c r="Y22" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="Z22" s="53" t="s">
+      <c r="Z22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AA22" s="54" t="s">
+      <c r="AA22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AB22" s="55" t="s">
+      <c r="AB22" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="AC22" s="56" t="s">
+      <c r="AC22" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AD22" s="57" t="s">
+      <c r="AD22" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AE22" s="58" t="s">
+      <c r="AE22" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="AF22" s="53" t="s">
+      <c r="AF22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AG22" s="54" t="s">
+      <c r="AG22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AH22" s="55" t="s">
+      <c r="AH22" s="54" t="s">
         <v>68</v>
       </c>
     </row>
@@ -11415,29 +11376,29 @@
         <f t="shared" si="1"/>
         <v>665.8</v>
       </c>
-      <c r="L23" s="60"/>
+      <c r="L23" s="58"/>
       <c r="M23" s="59"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="55"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="57"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="55"/>
-      <c r="AC23" s="56"/>
-      <c r="AD23" s="57"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="53"/>
-      <c r="AG23" s="54"/>
-      <c r="AH23" s="55"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="57"/>
+      <c r="Z23" s="52"/>
+      <c r="AA23" s="53"/>
+      <c r="AB23" s="54"/>
+      <c r="AC23" s="55"/>
+      <c r="AD23" s="56"/>
+      <c r="AE23" s="57"/>
+      <c r="AF23" s="52"/>
+      <c r="AG23" s="53"/>
+      <c r="AH23" s="54"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -12810,41 +12771,41 @@
         <v>67</v>
       </c>
       <c r="M42" s="59"/>
-      <c r="N42" s="52" t="s">
+      <c r="N42" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="46" t="s">
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="R42" s="46"/>
-      <c r="S42" s="46"/>
-      <c r="T42" s="52" t="s">
+      <c r="R42" s="48"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="46" t="s">
+      <c r="U42" s="60"/>
+      <c r="V42" s="60"/>
+      <c r="W42" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X42" s="46"/>
-      <c r="Y42" s="46"/>
-      <c r="Z42" s="52" t="s">
+      <c r="X42" s="48"/>
+      <c r="Y42" s="48"/>
+      <c r="Z42" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AA42" s="52"/>
-      <c r="AB42" s="52"/>
-      <c r="AC42" s="46" t="s">
+      <c r="AA42" s="60"/>
+      <c r="AB42" s="60"/>
+      <c r="AC42" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AD42" s="46"/>
-      <c r="AE42" s="46"/>
-      <c r="AF42" s="52" t="s">
+      <c r="AD42" s="48"/>
+      <c r="AE42" s="48"/>
+      <c r="AF42" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AG42" s="52"/>
-      <c r="AH42" s="52"/>
+      <c r="AG42" s="60"/>
+      <c r="AH42" s="60"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -12868,73 +12829,73 @@
         <f t="shared" si="1"/>
         <v>1005.61</v>
       </c>
-      <c r="L43" s="60" t="s">
+      <c r="L43" s="58" t="s">
         <v>65</v>
       </c>
       <c r="M43" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="N43" s="53" t="s">
+      <c r="N43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="54" t="s">
+      <c r="O43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="P43" s="55" t="s">
+      <c r="P43" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Q43" s="56" t="s">
+      <c r="Q43" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="R43" s="57" t="s">
+      <c r="R43" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="S43" s="58" t="s">
+      <c r="S43" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T43" s="53" t="s">
+      <c r="T43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U43" s="54" t="s">
+      <c r="U43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="V43" s="55" t="s">
+      <c r="V43" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="W43" s="56" t="s">
+      <c r="W43" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X43" s="57" t="s">
+      <c r="X43" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="Y43" s="58" t="s">
+      <c r="Y43" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="Z43" s="53" t="s">
+      <c r="Z43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AA43" s="54" t="s">
+      <c r="AA43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AB43" s="55" t="s">
+      <c r="AB43" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="AC43" s="56" t="s">
+      <c r="AC43" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AD43" s="57" t="s">
+      <c r="AD43" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AE43" s="58" t="s">
+      <c r="AE43" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="AF43" s="53" t="s">
+      <c r="AF43" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="AG43" s="54" t="s">
+      <c r="AG43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="AH43" s="55" t="s">
+      <c r="AH43" s="54" t="s">
         <v>68</v>
       </c>
     </row>
@@ -12960,29 +12921,29 @@
         <f t="shared" si="1"/>
         <v>1050.77</v>
       </c>
-      <c r="L44" s="60"/>
+      <c r="L44" s="58"/>
       <c r="M44" s="59"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="54"/>
-      <c r="P44" s="55"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="53"/>
-      <c r="U44" s="54"/>
-      <c r="V44" s="55"/>
-      <c r="W44" s="56"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="58"/>
-      <c r="Z44" s="53"/>
-      <c r="AA44" s="54"/>
-      <c r="AB44" s="55"/>
-      <c r="AC44" s="56"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="58"/>
-      <c r="AF44" s="53"/>
-      <c r="AG44" s="54"/>
-      <c r="AH44" s="55"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="55"/>
+      <c r="R44" s="56"/>
+      <c r="S44" s="57"/>
+      <c r="T44" s="52"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="54"/>
+      <c r="W44" s="55"/>
+      <c r="X44" s="56"/>
+      <c r="Y44" s="57"/>
+      <c r="Z44" s="52"/>
+      <c r="AA44" s="53"/>
+      <c r="AB44" s="54"/>
+      <c r="AC44" s="55"/>
+      <c r="AD44" s="56"/>
+      <c r="AE44" s="57"/>
+      <c r="AF44" s="52"/>
+      <c r="AG44" s="53"/>
+      <c r="AH44" s="54"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -14992,29 +14953,60 @@
     <sortCondition ref="C5:C48"/>
   </sortState>
   <mergeCells count="93">
-    <mergeCell ref="AF43:AF44"/>
-    <mergeCell ref="AG43:AG44"/>
-    <mergeCell ref="AH43:AH44"/>
-    <mergeCell ref="AA43:AA44"/>
-    <mergeCell ref="AB43:AB44"/>
-    <mergeCell ref="AC43:AC44"/>
-    <mergeCell ref="AD43:AD44"/>
-    <mergeCell ref="AE43:AE44"/>
-    <mergeCell ref="V43:V44"/>
-    <mergeCell ref="W43:W44"/>
-    <mergeCell ref="X43:X44"/>
-    <mergeCell ref="Y43:Y44"/>
-    <mergeCell ref="Z43:Z44"/>
-    <mergeCell ref="Q43:Q44"/>
-    <mergeCell ref="R43:R44"/>
-    <mergeCell ref="S43:S44"/>
-    <mergeCell ref="T43:T44"/>
-    <mergeCell ref="U43:U44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="Z21:AB21"/>
+    <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="AF21:AH21"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="V22:V23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="Z22:Z23"/>
     <mergeCell ref="AF22:AF23"/>
     <mergeCell ref="AG22:AG23"/>
     <mergeCell ref="AH22:AH23"/>
@@ -15031,60 +15023,29 @@
     <mergeCell ref="AC22:AC23"/>
     <mergeCell ref="AD22:AD23"/>
     <mergeCell ref="AE22:AE23"/>
-    <mergeCell ref="AF21:AH21"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="V22:V23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="Y22:Y23"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:Y21"/>
-    <mergeCell ref="Z21:AB21"/>
-    <mergeCell ref="AC21:AE21"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="Q43:Q44"/>
+    <mergeCell ref="R43:R44"/>
+    <mergeCell ref="S43:S44"/>
+    <mergeCell ref="T43:T44"/>
+    <mergeCell ref="U43:U44"/>
+    <mergeCell ref="V43:V44"/>
+    <mergeCell ref="W43:W44"/>
+    <mergeCell ref="X43:X44"/>
+    <mergeCell ref="Y43:Y44"/>
+    <mergeCell ref="Z43:Z44"/>
+    <mergeCell ref="AF43:AF44"/>
+    <mergeCell ref="AG43:AG44"/>
+    <mergeCell ref="AH43:AH44"/>
+    <mergeCell ref="AA43:AA44"/>
+    <mergeCell ref="AB43:AB44"/>
+    <mergeCell ref="AC43:AC44"/>
+    <mergeCell ref="AD43:AD44"/>
+    <mergeCell ref="AE43:AE44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15489,48 +15450,48 @@
       <c r="J4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="46" t="s">
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="48" t="s">
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="48"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="48"/>
-      <c r="W4" s="46" t="s">
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="48" t="s">
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="48"/>
-      <c r="AC4" s="48"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="46" t="s">
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF4" s="46"/>
-      <c r="AG4" s="46"/>
-      <c r="AH4" s="46"/>
-      <c r="AI4" s="48" t="s">
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="48"/>
-      <c r="AL4" s="48"/>
+      <c r="AJ4" s="46"/>
+      <c r="AK4" s="46"/>
+      <c r="AL4" s="46"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
@@ -15543,58 +15504,58 @@
         <v>41</v>
       </c>
       <c r="L5" s="47"/>
-      <c r="M5" s="51" t="s">
+      <c r="M5" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="51"/>
+      <c r="N5" s="49"/>
       <c r="O5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P5" s="50"/>
-      <c r="Q5" s="46" t="s">
+      <c r="Q5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="46"/>
+      <c r="R5" s="48"/>
       <c r="S5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T5" s="47"/>
-      <c r="U5" s="48" t="s">
+      <c r="U5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V5" s="48"/>
+      <c r="V5" s="46"/>
       <c r="W5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X5" s="50"/>
-      <c r="Y5" s="46" t="s">
+      <c r="Y5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="46"/>
+      <c r="Z5" s="48"/>
       <c r="AA5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB5" s="47"/>
-      <c r="AC5" s="48" t="s">
+      <c r="AC5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD5" s="48"/>
+      <c r="AD5" s="46"/>
       <c r="AE5" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF5" s="50"/>
-      <c r="AG5" s="46" t="s">
+      <c r="AG5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH5" s="46"/>
+      <c r="AH5" s="48"/>
       <c r="AI5" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ5" s="47"/>
-      <c r="AK5" s="48" t="s">
+      <c r="AK5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL5" s="48"/>
+      <c r="AL5" s="46"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J6" s="8" t="s">
@@ -15686,13 +15647,13 @@
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="51"/>
       <c r="I7">
         <v>0</v>
       </c>
@@ -15792,7 +15753,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="51"/>
       <c r="C8" t="s">
         <v>39</v>
       </c>
@@ -18939,48 +18900,48 @@
       <c r="J43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K43" s="48" t="s">
+      <c r="K43" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="46" t="s">
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P43" s="46"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="46"/>
-      <c r="S43" s="48" t="s">
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-      <c r="V43" s="48"/>
-      <c r="W43" s="46" t="s">
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X43" s="46"/>
-      <c r="Y43" s="46"/>
-      <c r="Z43" s="46"/>
-      <c r="AA43" s="48" t="s">
+      <c r="X43" s="48"/>
+      <c r="Y43" s="48"/>
+      <c r="Z43" s="48"/>
+      <c r="AA43" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB43" s="48"/>
-      <c r="AC43" s="48"/>
-      <c r="AD43" s="48"/>
-      <c r="AE43" s="46" t="s">
+      <c r="AB43" s="46"/>
+      <c r="AC43" s="46"/>
+      <c r="AD43" s="46"/>
+      <c r="AE43" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF43" s="46"/>
-      <c r="AG43" s="46"/>
-      <c r="AH43" s="46"/>
-      <c r="AI43" s="48" t="s">
+      <c r="AF43" s="48"/>
+      <c r="AG43" s="48"/>
+      <c r="AH43" s="48"/>
+      <c r="AI43" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ43" s="48"/>
-      <c r="AK43" s="48"/>
-      <c r="AL43" s="48"/>
+      <c r="AJ43" s="46"/>
+      <c r="AK43" s="46"/>
+      <c r="AL43" s="46"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
@@ -18993,58 +18954,58 @@
         <v>41</v>
       </c>
       <c r="L44" s="47"/>
-      <c r="M44" s="51" t="s">
+      <c r="M44" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N44" s="51"/>
+      <c r="N44" s="49"/>
       <c r="O44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P44" s="50"/>
-      <c r="Q44" s="46" t="s">
+      <c r="Q44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R44" s="46"/>
+      <c r="R44" s="48"/>
       <c r="S44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T44" s="47"/>
-      <c r="U44" s="48" t="s">
+      <c r="U44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V44" s="48"/>
+      <c r="V44" s="46"/>
       <c r="W44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X44" s="50"/>
-      <c r="Y44" s="46" t="s">
+      <c r="Y44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z44" s="46"/>
+      <c r="Z44" s="48"/>
       <c r="AA44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB44" s="47"/>
-      <c r="AC44" s="48" t="s">
+      <c r="AC44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD44" s="48"/>
+      <c r="AD44" s="46"/>
       <c r="AE44" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF44" s="50"/>
-      <c r="AG44" s="46" t="s">
+      <c r="AG44" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH44" s="46"/>
+      <c r="AH44" s="48"/>
       <c r="AI44" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ44" s="47"/>
-      <c r="AK44" s="48" t="s">
+      <c r="AK44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL44" s="48"/>
+      <c r="AL44" s="46"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J45" s="8" t="s">
@@ -19136,13 +19097,13 @@
       </c>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="49" t="s">
+      <c r="C46" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="49"/>
+      <c r="D46" s="51"/>
       <c r="I46">
         <v>0</v>
       </c>
@@ -19242,7 +19203,7 @@
       </c>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B47" s="49"/>
+      <c r="B47" s="51"/>
       <c r="C47" t="s">
         <v>39</v>
       </c>
@@ -22297,48 +22258,48 @@
       <c r="J83" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K83" s="48" t="s">
+      <c r="K83" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L83" s="48"/>
-      <c r="M83" s="48"/>
-      <c r="N83" s="48"/>
-      <c r="O83" s="46" t="s">
+      <c r="L83" s="46"/>
+      <c r="M83" s="46"/>
+      <c r="N83" s="46"/>
+      <c r="O83" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P83" s="46"/>
-      <c r="Q83" s="46"/>
-      <c r="R83" s="46"/>
-      <c r="S83" s="48" t="s">
+      <c r="P83" s="48"/>
+      <c r="Q83" s="48"/>
+      <c r="R83" s="48"/>
+      <c r="S83" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T83" s="48"/>
-      <c r="U83" s="48"/>
-      <c r="V83" s="48"/>
-      <c r="W83" s="46" t="s">
+      <c r="T83" s="46"/>
+      <c r="U83" s="46"/>
+      <c r="V83" s="46"/>
+      <c r="W83" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="X83" s="46"/>
-      <c r="Y83" s="46"/>
-      <c r="Z83" s="46"/>
-      <c r="AA83" s="48" t="s">
+      <c r="X83" s="48"/>
+      <c r="Y83" s="48"/>
+      <c r="Z83" s="48"/>
+      <c r="AA83" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AB83" s="48"/>
-      <c r="AC83" s="48"/>
-      <c r="AD83" s="48"/>
-      <c r="AE83" s="46" t="s">
+      <c r="AB83" s="46"/>
+      <c r="AC83" s="46"/>
+      <c r="AD83" s="46"/>
+      <c r="AE83" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AF83" s="46"/>
-      <c r="AG83" s="46"/>
-      <c r="AH83" s="46"/>
-      <c r="AI83" s="48" t="s">
+      <c r="AF83" s="48"/>
+      <c r="AG83" s="48"/>
+      <c r="AH83" s="48"/>
+      <c r="AI83" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ83" s="48"/>
-      <c r="AK83" s="48"/>
-      <c r="AL83" s="48"/>
+      <c r="AJ83" s="46"/>
+      <c r="AK83" s="46"/>
+      <c r="AL83" s="46"/>
     </row>
     <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H84" t="s">
@@ -22351,58 +22312,58 @@
         <v>41</v>
       </c>
       <c r="L84" s="47"/>
-      <c r="M84" s="51" t="s">
+      <c r="M84" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="N84" s="51"/>
+      <c r="N84" s="49"/>
       <c r="O84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="P84" s="50"/>
-      <c r="Q84" s="46" t="s">
+      <c r="Q84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R84" s="46"/>
+      <c r="R84" s="48"/>
       <c r="S84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="T84" s="47"/>
-      <c r="U84" s="48" t="s">
+      <c r="U84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V84" s="48"/>
+      <c r="V84" s="46"/>
       <c r="W84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="X84" s="50"/>
-      <c r="Y84" s="46" t="s">
+      <c r="Y84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Z84" s="46"/>
+      <c r="Z84" s="48"/>
       <c r="AA84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AB84" s="47"/>
-      <c r="AC84" s="48" t="s">
+      <c r="AC84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AD84" s="48"/>
+      <c r="AD84" s="46"/>
       <c r="AE84" s="50" t="s">
         <v>41</v>
       </c>
       <c r="AF84" s="50"/>
-      <c r="AG84" s="46" t="s">
+      <c r="AG84" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AH84" s="46"/>
+      <c r="AH84" s="48"/>
       <c r="AI84" s="47" t="s">
         <v>41</v>
       </c>
       <c r="AJ84" s="47"/>
-      <c r="AK84" s="48" t="s">
+      <c r="AK84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AL84" s="48"/>
+      <c r="AL84" s="46"/>
     </row>
     <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="J85" s="8" t="s">
@@ -22494,13 +22455,13 @@
       </c>
     </row>
     <row r="86" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B86" s="49" t="s">
+      <c r="B86" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C86" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D86" s="49"/>
+      <c r="D86" s="51"/>
       <c r="I86">
         <v>0</v>
       </c>
@@ -22600,7 +22561,7 @@
       </c>
     </row>
     <row r="87" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B87" s="49"/>
+      <c r="B87" s="51"/>
       <c r="C87" t="s">
         <v>39</v>
       </c>
@@ -25654,6 +25615,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="AI84:AJ84"/>
+    <mergeCell ref="AK84:AL84"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="W83:Z83"/>
+    <mergeCell ref="AA83:AD83"/>
+    <mergeCell ref="AE83:AH83"/>
+    <mergeCell ref="AI83:AL83"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="O84:P84"/>
+    <mergeCell ref="Q84:R84"/>
+    <mergeCell ref="S84:T84"/>
+    <mergeCell ref="U84:V84"/>
+    <mergeCell ref="W84:X84"/>
+    <mergeCell ref="Y84:Z84"/>
+    <mergeCell ref="AA84:AB84"/>
+    <mergeCell ref="AC84:AD84"/>
+    <mergeCell ref="AE84:AF84"/>
+    <mergeCell ref="AG84:AH84"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="O83:R83"/>
+    <mergeCell ref="S83:V83"/>
+    <mergeCell ref="AE43:AH43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="W44:X44"/>
+    <mergeCell ref="Y44:Z44"/>
+    <mergeCell ref="AA44:AB44"/>
+    <mergeCell ref="AC44:AD44"/>
+    <mergeCell ref="AE44:AF44"/>
+    <mergeCell ref="AG44:AH44"/>
+    <mergeCell ref="AI44:AJ44"/>
+    <mergeCell ref="AK44:AL44"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="O43:R43"/>
+    <mergeCell ref="S43:V43"/>
+    <mergeCell ref="W43:Z43"/>
+    <mergeCell ref="AA43:AD43"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="AE4:AH4"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="AI4:AL4"/>
@@ -25670,59 +25684,6 @@
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="O43:R43"/>
-    <mergeCell ref="S43:V43"/>
-    <mergeCell ref="W43:Z43"/>
-    <mergeCell ref="AA43:AD43"/>
-    <mergeCell ref="AE43:AH43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="W44:X44"/>
-    <mergeCell ref="Y44:Z44"/>
-    <mergeCell ref="AA44:AB44"/>
-    <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="AE44:AF44"/>
-    <mergeCell ref="AG44:AH44"/>
-    <mergeCell ref="AI44:AJ44"/>
-    <mergeCell ref="AK44:AL44"/>
-    <mergeCell ref="AA84:AB84"/>
-    <mergeCell ref="AC84:AD84"/>
-    <mergeCell ref="AE84:AF84"/>
-    <mergeCell ref="AG84:AH84"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="O83:R83"/>
-    <mergeCell ref="S83:V83"/>
-    <mergeCell ref="AI84:AJ84"/>
-    <mergeCell ref="AK84:AL84"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="W83:Z83"/>
-    <mergeCell ref="AA83:AD83"/>
-    <mergeCell ref="AE83:AH83"/>
-    <mergeCell ref="AI83:AL83"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="O84:P84"/>
-    <mergeCell ref="Q84:R84"/>
-    <mergeCell ref="S84:T84"/>
-    <mergeCell ref="U84:V84"/>
-    <mergeCell ref="W84:X84"/>
-    <mergeCell ref="Y84:Z84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25733,7 +25694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="F41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AD50" sqref="AD50"/>
     </sheetView>
   </sheetViews>

</xml_diff>